<commit_message>
bugfix hough + clean up
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5339,82 +5339,82 @@
   <dimension ref="A1:DF59"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="4.140625" customWidth="true"/>
-    <col min="5" max="5" width="9.140625" customWidth="true"/>
-    <col min="6" max="6" width="5.7109375" customWidth="true"/>
-    <col min="7" max="7" width="2.140625" customWidth="true"/>
+    <col min="4" max="4" width="6.7109375" customWidth="true"/>
+    <col min="5" max="5" width="8.140625" customWidth="true"/>
+    <col min="6" max="6" width="7.7109375" customWidth="true"/>
+    <col min="7" max="7" width="5.7109375" customWidth="true"/>
     <col min="8" max="8" width="7.140625" customWidth="true"/>
-    <col min="9" max="9" width="5.7109375" customWidth="true"/>
-    <col min="10" max="10" width="4.140625" customWidth="true"/>
-    <col min="11" max="11" width="7.7109375" customWidth="true"/>
+    <col min="9" max="9" width="8.7109375" customWidth="true"/>
+    <col min="10" max="10" width="7.7109375" customWidth="true"/>
+    <col min="11" max="11" width="10.7109375" customWidth="true"/>
     <col min="1" max="1" width="13.5703125" customWidth="true"/>
-    <col min="15" max="15" width="5.7109375" customWidth="true"/>
+    <col min="15" max="15" width="4.140625" customWidth="true"/>
     <col min="16" max="16" width="8.140625" customWidth="true"/>
-    <col min="17" max="17" width="6.7109375" customWidth="true"/>
-    <col min="18" max="18" width="4.7109375" customWidth="true"/>
+    <col min="17" max="17" width="4.7109375" customWidth="true"/>
+    <col min="18" max="18" width="11.7109375" customWidth="true"/>
     <col min="19" max="19" width="7.140625" customWidth="true"/>
-    <col min="20" max="20" width="7.7109375" customWidth="true"/>
-    <col min="21" max="21" width="5.7109375" customWidth="true"/>
-    <col min="22" max="22" width="9.7109375" customWidth="true"/>
-    <col min="26" max="26" width="4.140625" customWidth="true"/>
-    <col min="27" max="27" width="9.140625" customWidth="true"/>
-    <col min="28" max="28" width="6.7109375" customWidth="true"/>
-    <col min="29" max="29" width="2.85546875" customWidth="true"/>
-    <col min="30" max="30" width="6.85546875" customWidth="true"/>
+    <col min="20" max="20" width="6.7109375" customWidth="true"/>
+    <col min="21" max="21" width="11.7109375" customWidth="true"/>
+    <col min="22" max="22" width="14.7109375" customWidth="true"/>
+    <col min="26" max="26" width="5.7109375" customWidth="true"/>
+    <col min="27" max="27" width="8.140625" customWidth="true"/>
+    <col min="28" max="28" width="7.7109375" customWidth="true"/>
+    <col min="29" max="29" width="4.42578125" customWidth="true"/>
+    <col min="30" max="30" width="7.85546875" customWidth="true"/>
     <col min="31" max="31" width="6.42578125" customWidth="true"/>
-    <col min="32" max="32" width="4.85546875" customWidth="true"/>
+    <col min="32" max="32" width="5.85546875" customWidth="true"/>
     <col min="33" max="33" width="8.42578125" customWidth="true"/>
-    <col min="37" max="37" width="4.140625" customWidth="true"/>
-    <col min="38" max="38" width="9.140625" customWidth="true"/>
+    <col min="37" max="37" width="5.7109375" customWidth="true"/>
+    <col min="38" max="38" width="8.140625" customWidth="true"/>
     <col min="39" max="39" width="6.7109375" customWidth="true"/>
-    <col min="40" max="40" width="2.140625" customWidth="true"/>
+    <col min="40" max="40" width="4.7109375" customWidth="true"/>
     <col min="41" max="41" width="7.140625" customWidth="true"/>
-    <col min="42" max="42" width="5.7109375" customWidth="true"/>
-    <col min="43" max="43" width="5.140625" customWidth="true"/>
-    <col min="44" max="44" width="7.7109375" customWidth="true"/>
-    <col min="48" max="48" width="4.140625" customWidth="true"/>
+    <col min="42" max="42" width="7.7109375" customWidth="true"/>
+    <col min="43" max="43" width="6.7109375" customWidth="true"/>
+    <col min="44" max="44" width="9.7109375" customWidth="true"/>
+    <col min="48" max="48" width="11.7109375" customWidth="true"/>
     <col min="49" max="49" width="8.140625" customWidth="true"/>
-    <col min="50" max="50" width="4.7109375" customWidth="true"/>
-    <col min="51" max="51" width="2.140625" customWidth="true"/>
+    <col min="50" max="50" width="7.7109375" customWidth="true"/>
+    <col min="51" max="51" width="11.7109375" customWidth="true"/>
     <col min="52" max="52" width="7.140625" customWidth="true"/>
-    <col min="53" max="53" width="4.7109375" customWidth="true"/>
-    <col min="54" max="54" width="5.140625" customWidth="true"/>
-    <col min="55" max="55" width="6.7109375" customWidth="true"/>
-    <col min="59" max="59" width="4.140625" customWidth="true"/>
+    <col min="53" max="53" width="8.7109375" customWidth="true"/>
+    <col min="54" max="54" width="11.7109375" customWidth="true"/>
+    <col min="55" max="55" width="14.7109375" customWidth="true"/>
+    <col min="59" max="59" width="6.7109375" customWidth="true"/>
     <col min="60" max="60" width="8.140625" customWidth="true"/>
-    <col min="61" max="61" width="4.7109375" customWidth="true"/>
-    <col min="62" max="62" width="5.7109375" customWidth="true"/>
+    <col min="61" max="61" width="7.7109375" customWidth="true"/>
+    <col min="62" max="62" width="11.7109375" customWidth="true"/>
     <col min="63" max="63" width="7.140625" customWidth="true"/>
-    <col min="64" max="64" width="8.7109375" customWidth="true"/>
-    <col min="65" max="65" width="6.7109375" customWidth="true"/>
-    <col min="66" max="66" width="10.7109375" customWidth="true"/>
-    <col min="70" max="70" width="3.140625" customWidth="true"/>
+    <col min="64" max="64" width="6.7109375" customWidth="true"/>
+    <col min="65" max="65" width="11.7109375" customWidth="true"/>
+    <col min="66" max="66" width="15.7109375" customWidth="true"/>
+    <col min="70" max="70" width="6.7109375" customWidth="true"/>
     <col min="71" max="71" width="8.140625" customWidth="true"/>
-    <col min="72" max="72" width="5.7109375" customWidth="true"/>
-    <col min="73" max="73" width="4.140625" customWidth="true"/>
-    <col min="74" max="74" width="9.140625" customWidth="true"/>
-    <col min="75" max="75" width="6.7109375" customWidth="true"/>
-    <col min="76" max="76" width="6.140625" customWidth="true"/>
-    <col min="77" max="77" width="7.7109375" customWidth="true"/>
-    <col min="81" max="81" width="5.7109375" customWidth="true"/>
+    <col min="72" max="72" width="8.7109375" customWidth="true"/>
+    <col min="73" max="73" width="12.7109375" customWidth="true"/>
+    <col min="74" max="74" width="7.140625" customWidth="true"/>
+    <col min="75" max="75" width="8.7109375" customWidth="true"/>
+    <col min="76" max="76" width="11.7109375" customWidth="true"/>
+    <col min="77" max="77" width="15.7109375" customWidth="true"/>
+    <col min="81" max="81" width="6.7109375" customWidth="true"/>
     <col min="82" max="82" width="8.140625" customWidth="true"/>
-    <col min="83" max="83" width="6.7109375" customWidth="true"/>
-    <col min="84" max="84" width="4.7109375" customWidth="true"/>
+    <col min="83" max="83" width="7.7109375" customWidth="true"/>
+    <col min="84" max="84" width="3.7109375" customWidth="true"/>
     <col min="85" max="85" width="7.140625" customWidth="true"/>
-    <col min="86" max="86" width="7.7109375" customWidth="true"/>
-    <col min="87" max="87" width="6.7109375" customWidth="true"/>
-    <col min="88" max="88" width="9.7109375" customWidth="true"/>
-    <col min="92" max="92" width="4.140625" customWidth="true"/>
+    <col min="86" max="86" width="6.7109375" customWidth="true"/>
+    <col min="87" max="87" width="5.140625" customWidth="true"/>
+    <col min="88" max="88" width="8.7109375" customWidth="true"/>
+    <col min="92" max="92" width="11.7109375" customWidth="true"/>
     <col min="93" max="93" width="8.140625" customWidth="true"/>
-    <col min="94" max="94" width="5.7109375" customWidth="true"/>
-    <col min="95" max="95" width="2.140625" customWidth="true"/>
+    <col min="94" max="94" width="7.7109375" customWidth="true"/>
+    <col min="95" max="95" width="11.7109375" customWidth="true"/>
     <col min="96" max="96" width="7.140625" customWidth="true"/>
-    <col min="97" max="97" width="5.7109375" customWidth="true"/>
-    <col min="98" max="98" width="5.140625" customWidth="true"/>
-    <col min="99" max="99" width="7.7109375" customWidth="true"/>
-    <col min="103" max="103" width="11.7109375" customWidth="true"/>
+    <col min="97" max="97" width="7.7109375" customWidth="true"/>
+    <col min="98" max="98" width="11.7109375" customWidth="true"/>
+    <col min="99" max="99" width="15.7109375" customWidth="true"/>
+    <col min="103" max="103" width="4.140625" customWidth="true"/>
     <col min="104" max="104" width="8.140625" customWidth="true"/>
-    <col min="105" max="105" width="4.7109375" customWidth="true"/>
+    <col min="105" max="105" width="5.7109375" customWidth="true"/>
     <col min="106" max="106" width="3.7109375" customWidth="true"/>
     <col min="107" max="107" width="7.140625" customWidth="true"/>
     <col min="108" max="108" width="6.7109375" customWidth="true"/>
@@ -5672,13 +5672,13 @@
         <v>117</v>
       </c>
       <c r="D2" s="0">
-        <v>191.375</v>
+        <v>191</v>
       </c>
       <c r="E2" s="0">
-        <v>14353125</v>
+        <v>14325000</v>
       </c>
       <c r="F2" s="0">
-        <v>14.353125</v>
+        <v>14.324999999999999</v>
       </c>
       <c r="G2" s="0">
         <v>0</v>
@@ -5696,13 +5696,13 @@
         <v>0</v>
       </c>
       <c r="O2" s="0">
-        <v>192.625</v>
+        <v>190</v>
       </c>
       <c r="P2" s="0">
-        <v>14446875</v>
+        <v>14250000</v>
       </c>
       <c r="Q2" s="0">
-        <v>14.446874999999999</v>
+        <v>14.25</v>
       </c>
       <c r="R2" s="0">
         <v>0</v>
@@ -5720,13 +5720,13 @@
         <v>0</v>
       </c>
       <c r="Z2" s="0">
-        <v>78.099999999999994</v>
+        <v>82.5</v>
       </c>
       <c r="AA2" s="0">
-        <v>5857500</v>
+        <v>6187500</v>
       </c>
       <c r="AB2" s="0">
-        <v>5.857499999999999</v>
+        <v>6.1875</v>
       </c>
       <c r="AC2" s="0">
         <v>0</v>
@@ -5744,13 +5744,13 @@
         <v>0</v>
       </c>
       <c r="AK2" s="0">
-        <v>190.83333333333331</v>
+        <v>189.69999999999999</v>
       </c>
       <c r="AL2" s="0">
-        <v>14312499.999999998</v>
+        <v>14227500</v>
       </c>
       <c r="AM2" s="0">
-        <v>14.312499999999998</v>
+        <v>14.227499999999999</v>
       </c>
       <c r="AN2" s="0">
         <v>0</v>
@@ -5768,13 +5768,13 @@
         <v>0</v>
       </c>
       <c r="AV2" s="0">
-        <v>185.5</v>
+        <v>184.09999999999999</v>
       </c>
       <c r="AW2" s="0">
-        <v>13912500</v>
+        <v>13807500</v>
       </c>
       <c r="AX2" s="0">
-        <v>13.9125</v>
+        <v>13.807499999999999</v>
       </c>
       <c r="AY2" s="0">
         <v>0</v>
@@ -5792,13 +5792,13 @@
         <v>0</v>
       </c>
       <c r="BG2" s="0">
-        <v>187.59999999999999</v>
+        <v>186.66666666666669</v>
       </c>
       <c r="BH2" s="0">
-        <v>14070000</v>
+        <v>14000000.000000002</v>
       </c>
       <c r="BI2" s="0">
-        <v>14.069999999999999</v>
+        <v>14.000000000000002</v>
       </c>
       <c r="BJ2" s="0">
         <v>0</v>
@@ -5816,13 +5816,13 @@
         <v>0</v>
       </c>
       <c r="BR2" s="0">
-        <v>82</v>
+        <v>81.375</v>
       </c>
       <c r="BS2" s="0">
-        <v>6150000</v>
+        <v>6103125</v>
       </c>
       <c r="BT2" s="0">
-        <v>6.1499999999999995</v>
+        <v>6.1031249999999995</v>
       </c>
       <c r="BU2" s="0">
         <v>0</v>
@@ -5840,13 +5840,13 @@
         <v>0</v>
       </c>
       <c r="CC2" s="0">
-        <v>175.5</v>
+        <v>179.75</v>
       </c>
       <c r="CD2" s="0">
-        <v>13162500</v>
+        <v>13481250</v>
       </c>
       <c r="CE2" s="0">
-        <v>13.1625</v>
+        <v>13.481249999999999</v>
       </c>
       <c r="CF2" s="0">
         <v>0</v>
@@ -5864,13 +5864,13 @@
         <v>0</v>
       </c>
       <c r="CN2" s="0">
-        <v>188.30000000000001</v>
+        <v>184.75</v>
       </c>
       <c r="CO2" s="0">
-        <v>14122500</v>
+        <v>13856250</v>
       </c>
       <c r="CP2" s="0">
-        <v>14.1225</v>
+        <v>13.856249999999999</v>
       </c>
       <c r="CQ2" s="0">
         <v>0</v>
@@ -5888,13 +5888,13 @@
         <v>0</v>
       </c>
       <c r="CY2" s="0">
-        <v>189.25</v>
+        <v>186.5</v>
       </c>
       <c r="CZ2" s="0">
-        <v>14193750</v>
+        <v>13987500</v>
       </c>
       <c r="DA2" s="0">
-        <v>14.19375</v>
+        <v>13.987499999999999</v>
       </c>
       <c r="DB2" s="0">
         <v>0</v>
@@ -6652,244 +6652,244 @@
         <v>237</v>
       </c>
       <c r="D7" s="0">
-        <v>180.19999999999999</v>
+        <v>178.25</v>
       </c>
       <c r="E7" s="0">
-        <v>13515000</v>
+        <v>13368750</v>
       </c>
       <c r="F7" s="0">
-        <v>13.514999999999999</v>
+        <v>13.36875</v>
       </c>
       <c r="G7" s="0">
-        <v>11.175000000000011</v>
+        <v>12.75</v>
       </c>
       <c r="H7" s="0">
-        <v>838125.00000000081</v>
+        <v>956250</v>
       </c>
       <c r="I7" s="0">
-        <v>0.83812500000000079</v>
+        <v>0.95624999999999993</v>
       </c>
       <c r="J7" s="0">
-        <v>2793.7500000000027</v>
+        <v>3187.5</v>
       </c>
       <c r="K7" s="0">
-        <v>0.0027937500000000028</v>
+        <v>0.0031874999999999998</v>
       </c>
       <c r="O7" s="0">
-        <v>168.875</v>
+        <v>170</v>
       </c>
       <c r="P7" s="0">
-        <v>12665625</v>
+        <v>12750000</v>
       </c>
       <c r="Q7" s="0">
-        <v>12.665625</v>
+        <v>12.75</v>
       </c>
       <c r="R7" s="0">
-        <v>23.75</v>
+        <v>20</v>
       </c>
       <c r="S7" s="0">
-        <v>1781250</v>
+        <v>1500000</v>
       </c>
       <c r="T7" s="0">
-        <v>1.78125</v>
+        <v>1.5</v>
       </c>
       <c r="U7" s="0">
-        <v>5937.5</v>
+        <v>5000</v>
       </c>
       <c r="V7" s="0">
-        <v>0.0059375000000000001</v>
+        <v>0.0050000000000000001</v>
       </c>
       <c r="Z7" s="0">
-        <v>79.599999999999994</v>
+        <v>78.625</v>
       </c>
       <c r="AA7" s="0">
-        <v>5970000</v>
+        <v>5896875</v>
       </c>
       <c r="AB7" s="0">
-        <v>5.9699999999999998</v>
+        <v>5.8968749999999996</v>
       </c>
       <c r="AC7" s="0">
-        <v>-1.5</v>
+        <v>3.875</v>
       </c>
       <c r="AD7" s="0">
-        <v>-112500</v>
+        <v>290625</v>
       </c>
       <c r="AE7" s="0">
-        <v>-0.11249999999999999</v>
+        <v>0.29062499999999997</v>
       </c>
       <c r="AF7" s="0">
-        <v>-375</v>
+        <v>968.75</v>
       </c>
       <c r="AG7" s="0">
-        <v>-0.00037499999999999995</v>
+        <v>0.00096874999999999988</v>
       </c>
       <c r="AK7" s="0">
-        <v>181.375</v>
+        <v>180.375</v>
       </c>
       <c r="AL7" s="0">
-        <v>13603125</v>
+        <v>13528125</v>
       </c>
       <c r="AM7" s="0">
-        <v>13.603125</v>
+        <v>13.528124999999999</v>
       </c>
       <c r="AN7" s="0">
-        <v>9.4583333333333144</v>
+        <v>9.3249999999999886</v>
       </c>
       <c r="AO7" s="0">
-        <v>709374.9999999986</v>
+        <v>699374.99999999919</v>
       </c>
       <c r="AP7" s="0">
-        <v>0.70937499999999853</v>
+        <v>0.69937499999999908</v>
       </c>
       <c r="AQ7" s="0">
-        <v>2364.5833333333285</v>
+        <v>2331.2499999999973</v>
       </c>
       <c r="AR7" s="0">
-        <v>0.0023645833333333284</v>
+        <v>0.002331249999999997</v>
       </c>
       <c r="AV7" s="0">
-        <v>177.375</v>
+        <v>177.75</v>
       </c>
       <c r="AW7" s="0">
-        <v>13303125</v>
+        <v>13331250</v>
       </c>
       <c r="AX7" s="0">
-        <v>13.303125</v>
+        <v>13.331249999999999</v>
       </c>
       <c r="AY7" s="0">
-        <v>8.125</v>
+        <v>6.3499999999999943</v>
       </c>
       <c r="AZ7" s="0">
-        <v>609375</v>
+        <v>476249.99999999959</v>
       </c>
       <c r="BA7" s="0">
-        <v>0.609375</v>
+        <v>0.47624999999999956</v>
       </c>
       <c r="BB7" s="0">
-        <v>2031.25</v>
+        <v>1587.4999999999986</v>
       </c>
       <c r="BC7" s="0">
-        <v>0.0020312500000000001</v>
+        <v>0.0015874999999999986</v>
       </c>
       <c r="BG7" s="0">
-        <v>171.66666666666669</v>
+        <v>172.5</v>
       </c>
       <c r="BH7" s="0">
-        <v>12875000.000000002</v>
+        <v>12937500</v>
       </c>
       <c r="BI7" s="0">
-        <v>12.875000000000002</v>
+        <v>12.9375</v>
       </c>
       <c r="BJ7" s="0">
-        <v>15.933333333333309</v>
+        <v>14.166666666666686</v>
       </c>
       <c r="BK7" s="0">
-        <v>1194999.9999999981</v>
+        <v>1062500.0000000014</v>
       </c>
       <c r="BL7" s="0">
-        <v>1.1949999999999981</v>
+        <v>1.0625000000000013</v>
       </c>
       <c r="BM7" s="0">
-        <v>3983.3333333333271</v>
+        <v>3541.6666666666715</v>
       </c>
       <c r="BN7" s="0">
-        <v>0.0039833333333333266</v>
+        <v>0.0035416666666666713</v>
       </c>
       <c r="BR7" s="0">
-        <v>79.25</v>
+        <v>81.625</v>
       </c>
       <c r="BS7" s="0">
-        <v>5943750</v>
+        <v>6121875</v>
       </c>
       <c r="BT7" s="0">
-        <v>5.9437499999999996</v>
+        <v>6.1218750000000002</v>
       </c>
       <c r="BU7" s="0">
-        <v>2.75</v>
+        <v>-0.25</v>
       </c>
       <c r="BV7" s="0">
-        <v>206250</v>
+        <v>-18750</v>
       </c>
       <c r="BW7" s="0">
-        <v>0.20624999999999999</v>
+        <v>-0.018749999999999999</v>
       </c>
       <c r="BX7" s="0">
-        <v>687.5</v>
+        <v>-62.5</v>
       </c>
       <c r="BY7" s="0">
-        <v>0.00068749999999999996</v>
+        <v>-6.2500000000000001e-05</v>
       </c>
       <c r="CC7" s="0">
-        <v>162.30000000000001</v>
+        <v>162.84999999999999</v>
       </c>
       <c r="CD7" s="0">
-        <v>12172500</v>
+        <v>12213750</v>
       </c>
       <c r="CE7" s="0">
-        <v>12.172500000000001</v>
+        <v>12.213749999999999</v>
       </c>
       <c r="CF7" s="0">
-        <v>13.199999999999989</v>
+        <v>16.900000000000006</v>
       </c>
       <c r="CG7" s="0">
-        <v>989999.99999999919</v>
+        <v>1267500.0000000005</v>
       </c>
       <c r="CH7" s="0">
-        <v>0.9899999999999991</v>
+        <v>1.2675000000000003</v>
       </c>
       <c r="CI7" s="0">
-        <v>3299.9999999999973</v>
+        <v>4225.0000000000018</v>
       </c>
       <c r="CJ7" s="0">
-        <v>0.0032999999999999969</v>
+        <v>0.0042250000000000013</v>
       </c>
       <c r="CN7" s="0">
-        <v>178.5</v>
+        <v>177.08333333333331</v>
       </c>
       <c r="CO7" s="0">
-        <v>13387500</v>
+        <v>13281249.999999998</v>
       </c>
       <c r="CP7" s="0">
-        <v>13.387499999999999</v>
+        <v>13.281249999999998</v>
       </c>
       <c r="CQ7" s="0">
-        <v>9.8000000000000114</v>
+        <v>7.6666666666666856</v>
       </c>
       <c r="CR7" s="0">
-        <v>735000.00000000081</v>
+        <v>575000.0000000014</v>
       </c>
       <c r="CS7" s="0">
-        <v>0.73500000000000087</v>
+        <v>0.5750000000000014</v>
       </c>
       <c r="CT7" s="0">
-        <v>2450.0000000000027</v>
+        <v>1916.6666666666713</v>
       </c>
       <c r="CU7" s="0">
-        <v>0.002450000000000003</v>
+        <v>0.0019166666666666713</v>
       </c>
       <c r="CY7" s="0">
-        <v>171.19999999999999</v>
+        <v>174.5</v>
       </c>
       <c r="CZ7" s="0">
-        <v>12840000</v>
+        <v>13087500</v>
       </c>
       <c r="DA7" s="0">
-        <v>12.839999999999998</v>
+        <v>13.0875</v>
       </c>
       <c r="DB7" s="0">
-        <v>18.050000000000011</v>
+        <v>12</v>
       </c>
       <c r="DC7" s="0">
-        <v>1353750.0000000009</v>
+        <v>900000</v>
       </c>
       <c r="DD7" s="0">
-        <v>1.3537500000000009</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="DE7" s="0">
-        <v>4512.5000000000027</v>
+        <v>3000</v>
       </c>
       <c r="DF7" s="0">
-        <v>0.0045125000000000026</v>
+        <v>0.0029999999999999996</v>
       </c>
     </row>
     <row r="8">
@@ -7632,244 +7632,244 @@
         <v>357</v>
       </c>
       <c r="D12" s="0">
-        <v>169.5</v>
+        <v>169.16666666666669</v>
       </c>
       <c r="E12" s="0">
-        <v>12712500</v>
+        <v>12687500.000000002</v>
       </c>
       <c r="F12" s="0">
-        <v>12.7125</v>
+        <v>12.687500000000002</v>
       </c>
       <c r="G12" s="0">
-        <v>10.699999999999989</v>
+        <v>9.0833333333333144</v>
       </c>
       <c r="H12" s="0">
-        <v>802499.99999999919</v>
+        <v>681249.9999999986</v>
       </c>
       <c r="I12" s="0">
-        <v>0.8024999999999991</v>
+        <v>0.68124999999999858</v>
       </c>
       <c r="J12" s="0">
-        <v>2674.9999999999973</v>
+        <v>2270.8333333333285</v>
       </c>
       <c r="K12" s="0">
-        <v>0.0026749999999999968</v>
+        <v>0.0022708333333333287</v>
       </c>
       <c r="O12" s="0">
-        <v>160.66666666666666</v>
+        <v>159.55000000000001</v>
       </c>
       <c r="P12" s="0">
-        <v>12050000</v>
+        <v>11966250</v>
       </c>
       <c r="Q12" s="0">
-        <v>12.049999999999999</v>
+        <v>11.96625</v>
       </c>
       <c r="R12" s="0">
-        <v>8.2083333333333428</v>
+        <v>10.449999999999989</v>
       </c>
       <c r="S12" s="0">
-        <v>615625.0000000007</v>
+        <v>783749.99999999919</v>
       </c>
       <c r="T12" s="0">
-        <v>0.61562500000000064</v>
+        <v>0.78374999999999917</v>
       </c>
       <c r="U12" s="0">
-        <v>2052.0833333333358</v>
+        <v>2612.4999999999973</v>
       </c>
       <c r="V12" s="0">
-        <v>0.0020520833333333354</v>
+        <v>0.0026124999999999972</v>
       </c>
       <c r="Z12" s="0">
-        <v>74.666666666666657</v>
+        <v>75</v>
       </c>
       <c r="AA12" s="0">
-        <v>5599999.9999999991</v>
+        <v>5625000</v>
       </c>
       <c r="AB12" s="0">
-        <v>5.5999999999999988</v>
+        <v>5.625</v>
       </c>
       <c r="AC12" s="0">
-        <v>4.9333333333333371</v>
+        <v>3.625</v>
       </c>
       <c r="AD12" s="0">
-        <v>370000.00000000029</v>
+        <v>271875</v>
       </c>
       <c r="AE12" s="0">
-        <v>0.37000000000000027</v>
+        <v>0.27187499999999998</v>
       </c>
       <c r="AF12" s="0">
-        <v>1233.3333333333344</v>
+        <v>906.25</v>
       </c>
       <c r="AG12" s="0">
-        <v>0.0012333333333333343</v>
+        <v>0.00090624999999999994</v>
       </c>
       <c r="AK12" s="0">
-        <v>171.5</v>
+        <v>170</v>
       </c>
       <c r="AL12" s="0">
-        <v>12862500</v>
+        <v>12750000</v>
       </c>
       <c r="AM12" s="0">
-        <v>12.862499999999999</v>
+        <v>12.75</v>
       </c>
       <c r="AN12" s="0">
-        <v>9.875</v>
+        <v>10.375</v>
       </c>
       <c r="AO12" s="0">
-        <v>740625</v>
+        <v>778125</v>
       </c>
       <c r="AP12" s="0">
-        <v>0.74062499999999998</v>
+        <v>0.77812499999999996</v>
       </c>
       <c r="AQ12" s="0">
-        <v>2468.75</v>
+        <v>2593.75</v>
       </c>
       <c r="AR12" s="0">
-        <v>0.00246875</v>
+        <v>0.0025937499999999997</v>
       </c>
       <c r="AV12" s="0">
-        <v>171.16666666666669</v>
+        <v>170.5</v>
       </c>
       <c r="AW12" s="0">
-        <v>12837500.000000002</v>
+        <v>12787500</v>
       </c>
       <c r="AX12" s="0">
-        <v>12.8375</v>
+        <v>12.7875</v>
       </c>
       <c r="AY12" s="0">
-        <v>6.2083333333333144</v>
+        <v>7.25</v>
       </c>
       <c r="AZ12" s="0">
-        <v>465624.9999999986</v>
+        <v>543750</v>
       </c>
       <c r="BA12" s="0">
-        <v>0.46562499999999857</v>
+        <v>0.54374999999999996</v>
       </c>
       <c r="BB12" s="0">
-        <v>1552.0833333333287</v>
+        <v>1812.5</v>
       </c>
       <c r="BC12" s="0">
-        <v>0.0015520833333333285</v>
+        <v>0.0018124999999999999</v>
       </c>
       <c r="BG12" s="0">
-        <v>160.5</v>
+        <v>160.16666666666669</v>
       </c>
       <c r="BH12" s="0">
-        <v>12037500</v>
+        <v>12012500.000000002</v>
       </c>
       <c r="BI12" s="0">
-        <v>12.0375</v>
+        <v>12.012500000000001</v>
       </c>
       <c r="BJ12" s="0">
-        <v>11.166666666666686</v>
+        <v>12.333333333333314</v>
       </c>
       <c r="BK12" s="0">
-        <v>837500.0000000014</v>
+        <v>924999.9999999986</v>
       </c>
       <c r="BL12" s="0">
-        <v>0.83750000000000135</v>
+        <v>0.92499999999999849</v>
       </c>
       <c r="BM12" s="0">
-        <v>2791.6666666666715</v>
+        <v>3083.3333333333285</v>
       </c>
       <c r="BN12" s="0">
-        <v>0.002791666666666671</v>
+        <v>0.0030833333333333281</v>
       </c>
       <c r="BR12" s="0">
-        <v>79.083333333333343</v>
+        <v>79.25</v>
       </c>
       <c r="BS12" s="0">
-        <v>5931250.0000000009</v>
+        <v>5943750</v>
       </c>
       <c r="BT12" s="0">
-        <v>5.9312500000000004</v>
+        <v>5.9437499999999996</v>
       </c>
       <c r="BU12" s="0">
-        <v>0.16666666666665719</v>
+        <v>2.375</v>
       </c>
       <c r="BV12" s="0">
-        <v>12499.999999999289</v>
+        <v>178125</v>
       </c>
       <c r="BW12" s="0">
-        <v>0.012499999999999289</v>
+        <v>0.17812500000000001</v>
       </c>
       <c r="BX12" s="0">
-        <v>41.666666666664298</v>
+        <v>593.75</v>
       </c>
       <c r="BY12" s="0">
-        <v>4.16666666666643e-05</v>
+        <v>0.00059374999999999999</v>
       </c>
       <c r="CC12" s="0">
-        <v>152.625</v>
+        <v>151.58333333333331</v>
       </c>
       <c r="CD12" s="0">
-        <v>11446875</v>
+        <v>11368749.999999998</v>
       </c>
       <c r="CE12" s="0">
-        <v>11.446875</v>
+        <v>11.368749999999999</v>
       </c>
       <c r="CF12" s="0">
-        <v>9.6750000000000114</v>
+        <v>11.26666666666668</v>
       </c>
       <c r="CG12" s="0">
-        <v>725625.00000000081</v>
+        <v>845000.00000000105</v>
       </c>
       <c r="CH12" s="0">
-        <v>0.72562500000000085</v>
+        <v>0.84500000000000097</v>
       </c>
       <c r="CI12" s="0">
-        <v>2418.7500000000027</v>
+        <v>2816.6666666666702</v>
       </c>
       <c r="CJ12" s="0">
-        <v>0.0024187500000000029</v>
+        <v>0.00281666666666667</v>
       </c>
       <c r="CN12" s="0">
-        <v>167.09999999999999</v>
+        <v>168.33333333333331</v>
       </c>
       <c r="CO12" s="0">
-        <v>12532500</v>
+        <v>12624999.999999998</v>
       </c>
       <c r="CP12" s="0">
-        <v>12.532499999999999</v>
+        <v>12.624999999999998</v>
       </c>
       <c r="CQ12" s="0">
-        <v>11.400000000000006</v>
+        <v>8.75</v>
       </c>
       <c r="CR12" s="0">
-        <v>855000.00000000047</v>
+        <v>656250</v>
       </c>
       <c r="CS12" s="0">
-        <v>0.85500000000000043</v>
+        <v>0.65625</v>
       </c>
       <c r="CT12" s="0">
-        <v>2850.0000000000014</v>
+        <v>2187.5</v>
       </c>
       <c r="CU12" s="0">
-        <v>0.0028500000000000014</v>
+        <v>0.0021875000000000002</v>
       </c>
       <c r="CY12" s="0">
-        <v>160.33333333333331</v>
+        <v>161.25</v>
       </c>
       <c r="CZ12" s="0">
-        <v>12024999.999999998</v>
+        <v>12093750</v>
       </c>
       <c r="DA12" s="0">
-        <v>12.024999999999999</v>
+        <v>12.09375</v>
       </c>
       <c r="DB12" s="0">
-        <v>10.866666666666674</v>
+        <v>13.25</v>
       </c>
       <c r="DC12" s="0">
-        <v>815000.00000000058</v>
+        <v>993750</v>
       </c>
       <c r="DD12" s="0">
-        <v>0.8150000000000005</v>
+        <v>0.99374999999999991</v>
       </c>
       <c r="DE12" s="0">
-        <v>2716.6666666666688</v>
+        <v>3312.5</v>
       </c>
       <c r="DF12" s="0">
-        <v>0.0027166666666666684</v>
+        <v>0.0033124999999999999</v>
       </c>
     </row>
     <row r="13">
@@ -8612,244 +8612,244 @@
         <v>477</v>
       </c>
       <c r="D17" s="0">
-        <v>164.125</v>
+        <v>160.33333333333331</v>
       </c>
       <c r="E17" s="0">
-        <v>12309375</v>
+        <v>12024999.999999998</v>
       </c>
       <c r="F17" s="0">
-        <v>12.309374999999999</v>
+        <v>12.024999999999999</v>
       </c>
       <c r="G17" s="0">
-        <v>5.375</v>
+        <v>8.8333333333333712</v>
       </c>
       <c r="H17" s="0">
-        <v>403125</v>
+        <v>662500.00000000279</v>
       </c>
       <c r="I17" s="0">
-        <v>0.40312500000000001</v>
+        <v>0.66250000000000286</v>
       </c>
       <c r="J17" s="0">
-        <v>1343.75</v>
+        <v>2208.3333333333426</v>
       </c>
       <c r="K17" s="0">
-        <v>0.0013437500000000001</v>
+        <v>0.002208333333333343</v>
       </c>
       <c r="O17" s="0">
-        <v>154.625</v>
+        <v>152.84999999999999</v>
       </c>
       <c r="P17" s="0">
-        <v>11596875</v>
+        <v>11463750</v>
       </c>
       <c r="Q17" s="0">
-        <v>11.596874999999999</v>
+        <v>11.463749999999999</v>
       </c>
       <c r="R17" s="0">
-        <v>6.0416666666666572</v>
+        <v>6.7000000000000171</v>
       </c>
       <c r="S17" s="0">
-        <v>453124.9999999993</v>
+        <v>502500.00000000128</v>
       </c>
       <c r="T17" s="0">
-        <v>0.45312499999999928</v>
+        <v>0.50250000000000128</v>
       </c>
       <c r="U17" s="0">
-        <v>1510.4166666666642</v>
+        <v>1675.0000000000043</v>
       </c>
       <c r="V17" s="0">
-        <v>0.0015104166666666642</v>
+        <v>0.0016750000000000042</v>
       </c>
       <c r="Z17" s="0">
-        <v>71.833333333333343</v>
+        <v>74.625</v>
       </c>
       <c r="AA17" s="0">
-        <v>5387500.0000000009</v>
+        <v>5596875</v>
       </c>
       <c r="AB17" s="0">
-        <v>5.3875000000000002</v>
+        <v>5.5968749999999998</v>
       </c>
       <c r="AC17" s="0">
-        <v>2.8333333333333144</v>
+        <v>0.375</v>
       </c>
       <c r="AD17" s="0">
-        <v>212499.99999999857</v>
+        <v>28125</v>
       </c>
       <c r="AE17" s="0">
-        <v>0.21249999999999858</v>
+        <v>0.028124999999999997</v>
       </c>
       <c r="AF17" s="0">
-        <v>708.3333333333286</v>
+        <v>93.75</v>
       </c>
       <c r="AG17" s="0">
-        <v>0.00070833333333332861</v>
+        <v>9.3749999999999988e-05</v>
       </c>
       <c r="AK17" s="0">
-        <v>163.5</v>
+        <v>162.25</v>
       </c>
       <c r="AL17" s="0">
-        <v>12262500</v>
+        <v>12168750</v>
       </c>
       <c r="AM17" s="0">
-        <v>12.262499999999999</v>
+        <v>12.168749999999999</v>
       </c>
       <c r="AN17" s="0">
-        <v>8</v>
+        <v>7.75</v>
       </c>
       <c r="AO17" s="0">
-        <v>600000</v>
+        <v>581250</v>
       </c>
       <c r="AP17" s="0">
-        <v>0.59999999999999998</v>
+        <v>0.58124999999999993</v>
       </c>
       <c r="AQ17" s="0">
-        <v>2000</v>
+        <v>1937.5</v>
       </c>
       <c r="AR17" s="0">
-        <v>0.002</v>
+        <v>0.0019374999999999998</v>
       </c>
       <c r="AV17" s="0">
-        <v>162.875</v>
+        <v>162.08333333333331</v>
       </c>
       <c r="AW17" s="0">
-        <v>12215625</v>
+        <v>12156249.999999998</v>
       </c>
       <c r="AX17" s="0">
-        <v>12.215624999999999</v>
+        <v>12.156249999999998</v>
       </c>
       <c r="AY17" s="0">
-        <v>8.2916666666666856</v>
+        <v>8.4166666666666856</v>
       </c>
       <c r="AZ17" s="0">
-        <v>621875.0000000014</v>
+        <v>631250.0000000014</v>
       </c>
       <c r="BA17" s="0">
-        <v>0.6218750000000014</v>
+        <v>0.63125000000000142</v>
       </c>
       <c r="BB17" s="0">
-        <v>2072.9166666666715</v>
+        <v>2104.1666666666715</v>
       </c>
       <c r="BC17" s="0">
-        <v>0.0020729166666666713</v>
+        <v>0.0021041666666666713</v>
       </c>
       <c r="BG17" s="0">
-        <v>157.875</v>
+        <v>156.625</v>
       </c>
       <c r="BH17" s="0">
-        <v>11840625</v>
+        <v>11746875</v>
       </c>
       <c r="BI17" s="0">
-        <v>11.840624999999999</v>
+        <v>11.746874999999999</v>
       </c>
       <c r="BJ17" s="0">
-        <v>2.625</v>
+        <v>3.5416666666666856</v>
       </c>
       <c r="BK17" s="0">
-        <v>196875</v>
+        <v>265625.0000000014</v>
       </c>
       <c r="BL17" s="0">
-        <v>0.19687499999999999</v>
+        <v>0.26562500000000139</v>
       </c>
       <c r="BM17" s="0">
-        <v>656.25</v>
+        <v>885.41666666667129</v>
       </c>
       <c r="BN17" s="0">
-        <v>0.00065624999999999993</v>
+        <v>0.00088541666666667128</v>
       </c>
       <c r="BR17" s="0">
-        <v>73</v>
+        <v>72.625</v>
       </c>
       <c r="BS17" s="0">
-        <v>5475000</v>
+        <v>5446875</v>
       </c>
       <c r="BT17" s="0">
-        <v>5.4749999999999996</v>
+        <v>5.4468749999999995</v>
       </c>
       <c r="BU17" s="0">
-        <v>6.0833333333333428</v>
+        <v>6.625</v>
       </c>
       <c r="BV17" s="0">
-        <v>456250.0000000007</v>
+        <v>496875</v>
       </c>
       <c r="BW17" s="0">
-        <v>0.45625000000000071</v>
+        <v>0.49687499999999996</v>
       </c>
       <c r="BX17" s="0">
-        <v>1520.8333333333358</v>
+        <v>1656.25</v>
       </c>
       <c r="BY17" s="0">
-        <v>0.0015208333333333356</v>
+        <v>0.00165625</v>
       </c>
       <c r="CC17" s="0">
-        <v>145.625</v>
+        <v>144.875</v>
       </c>
       <c r="CD17" s="0">
-        <v>10921875</v>
+        <v>10865625</v>
       </c>
       <c r="CE17" s="0">
-        <v>10.921875</v>
+        <v>10.865625</v>
       </c>
       <c r="CF17" s="0">
-        <v>7</v>
+        <v>6.7083333333333144</v>
       </c>
       <c r="CG17" s="0">
-        <v>525000</v>
+        <v>503124.9999999986</v>
       </c>
       <c r="CH17" s="0">
-        <v>0.52500000000000002</v>
+        <v>0.5031249999999986</v>
       </c>
       <c r="CI17" s="0">
-        <v>1750</v>
+        <v>1677.0833333333287</v>
       </c>
       <c r="CJ17" s="0">
-        <v>0.00175</v>
+        <v>0.0016770833333333286</v>
       </c>
       <c r="CN17" s="0">
-        <v>159.25</v>
+        <v>158.16666666666669</v>
       </c>
       <c r="CO17" s="0">
-        <v>11943750</v>
+        <v>11862500.000000002</v>
       </c>
       <c r="CP17" s="0">
-        <v>11.94375</v>
+        <v>11.862500000000001</v>
       </c>
       <c r="CQ17" s="0">
-        <v>7.8499999999999943</v>
+        <v>10.166666666666629</v>
       </c>
       <c r="CR17" s="0">
-        <v>588749.99999999953</v>
+        <v>762499.99999999721</v>
       </c>
       <c r="CS17" s="0">
-        <v>0.58874999999999955</v>
+        <v>0.76249999999999718</v>
       </c>
       <c r="CT17" s="0">
-        <v>1962.4999999999984</v>
+        <v>2541.6666666666574</v>
       </c>
       <c r="CU17" s="0">
-        <v>0.0019624999999999985</v>
+        <v>0.0025416666666666574</v>
       </c>
       <c r="CY17" s="0">
-        <v>155.625</v>
+        <v>155.83333333333331</v>
       </c>
       <c r="CZ17" s="0">
-        <v>11671875</v>
+        <v>11687499.999999998</v>
       </c>
       <c r="DA17" s="0">
-        <v>11.671875</v>
+        <v>11.687499999999998</v>
       </c>
       <c r="DB17" s="0">
-        <v>4.7083333333333144</v>
+        <v>5.4166666666666856</v>
       </c>
       <c r="DC17" s="0">
-        <v>353124.9999999986</v>
+        <v>406250.0000000014</v>
       </c>
       <c r="DD17" s="0">
-        <v>0.35312499999999858</v>
+        <v>0.40625000000000139</v>
       </c>
       <c r="DE17" s="0">
-        <v>1177.0833333333287</v>
+        <v>1354.1666666666713</v>
       </c>
       <c r="DF17" s="0">
-        <v>0.0011770833333333286</v>
+        <v>0.0013541666666666713</v>
       </c>
     </row>
     <row r="18">
@@ -9592,244 +9592,244 @@
         <v>597</v>
       </c>
       <c r="D22" s="0">
-        <v>154.375</v>
+        <v>154</v>
       </c>
       <c r="E22" s="0">
-        <v>11578125</v>
+        <v>11550000</v>
       </c>
       <c r="F22" s="0">
-        <v>11.578125</v>
+        <v>11.549999999999999</v>
       </c>
       <c r="G22" s="0">
-        <v>9.75</v>
+        <v>6.3333333333333144</v>
       </c>
       <c r="H22" s="0">
-        <v>731250</v>
+        <v>474999.9999999986</v>
       </c>
       <c r="I22" s="0">
-        <v>0.73124999999999996</v>
+        <v>0.47499999999999853</v>
       </c>
       <c r="J22" s="0">
-        <v>2437.5</v>
+        <v>1583.3333333333287</v>
       </c>
       <c r="K22" s="0">
-        <v>0.0024375</v>
+        <v>0.0015833333333333285</v>
       </c>
       <c r="O22" s="0">
-        <v>152.125</v>
+        <v>149</v>
       </c>
       <c r="P22" s="0">
-        <v>11409375</v>
+        <v>11175000</v>
       </c>
       <c r="Q22" s="0">
-        <v>11.409374999999999</v>
+        <v>11.174999999999999</v>
       </c>
       <c r="R22" s="0">
-        <v>2.5</v>
+        <v>3.8499999999999943</v>
       </c>
       <c r="S22" s="0">
-        <v>187500</v>
+        <v>288749.99999999959</v>
       </c>
       <c r="T22" s="0">
-        <v>0.1875</v>
+        <v>0.28874999999999956</v>
       </c>
       <c r="U22" s="0">
-        <v>625</v>
+        <v>962.49999999999864</v>
       </c>
       <c r="V22" s="0">
-        <v>0.00062500000000000001</v>
+        <v>0.00096249999999999851</v>
       </c>
       <c r="Z22" s="0">
-        <v>72.375</v>
+        <v>70</v>
       </c>
       <c r="AA22" s="0">
-        <v>5428125</v>
+        <v>5250000</v>
       </c>
       <c r="AB22" s="0">
-        <v>5.4281249999999996</v>
+        <v>5.25</v>
       </c>
       <c r="AC22" s="0">
-        <v>-0.54166666666665719</v>
+        <v>4.625</v>
       </c>
       <c r="AD22" s="0">
-        <v>-40624.999999999287</v>
+        <v>346875</v>
       </c>
       <c r="AE22" s="0">
-        <v>-0.040624999999999287</v>
+        <v>0.34687499999999999</v>
       </c>
       <c r="AF22" s="0">
-        <v>-135.4166666666643</v>
+        <v>1156.25</v>
       </c>
       <c r="AG22" s="0">
-        <v>-0.0001354166666666643</v>
+        <v>0.0011562499999999999</v>
       </c>
       <c r="AK22" s="0">
-        <v>156.16666666666669</v>
+        <v>155.08333333333331</v>
       </c>
       <c r="AL22" s="0">
-        <v>11712500.000000002</v>
+        <v>11631249.999999998</v>
       </c>
       <c r="AM22" s="0">
-        <v>11.7125</v>
+        <v>11.631249999999998</v>
       </c>
       <c r="AN22" s="0">
-        <v>7.3333333333333144</v>
+        <v>7.1666666666666856</v>
       </c>
       <c r="AO22" s="0">
-        <v>549999.9999999986</v>
+        <v>537500.0000000014</v>
       </c>
       <c r="AP22" s="0">
-        <v>0.5499999999999986</v>
+        <v>0.53750000000000142</v>
       </c>
       <c r="AQ22" s="0">
-        <v>1833.3333333333287</v>
+        <v>1791.6666666666713</v>
       </c>
       <c r="AR22" s="0">
-        <v>0.0018333333333333287</v>
+        <v>0.0017916666666666714</v>
       </c>
       <c r="AV22" s="0">
-        <v>158.16666666666669</v>
+        <v>157.41666666666669</v>
       </c>
       <c r="AW22" s="0">
-        <v>11862500.000000002</v>
+        <v>11806250.000000002</v>
       </c>
       <c r="AX22" s="0">
-        <v>11.862500000000001</v>
+        <v>11.80625</v>
       </c>
       <c r="AY22" s="0">
-        <v>4.7083333333333144</v>
+        <v>4.6666666666666288</v>
       </c>
       <c r="AZ22" s="0">
-        <v>353124.9999999986</v>
+        <v>349999.99999999715</v>
       </c>
       <c r="BA22" s="0">
-        <v>0.35312499999999858</v>
+        <v>0.34999999999999715</v>
       </c>
       <c r="BB22" s="0">
-        <v>1177.0833333333287</v>
+        <v>1166.6666666666572</v>
       </c>
       <c r="BC22" s="0">
-        <v>0.0011770833333333286</v>
+        <v>0.0011666666666666572</v>
       </c>
       <c r="BG22" s="0">
-        <v>146.875</v>
+        <v>146.25</v>
       </c>
       <c r="BH22" s="0">
-        <v>11015625</v>
+        <v>10968750</v>
       </c>
       <c r="BI22" s="0">
-        <v>11.015625</v>
+        <v>10.96875</v>
       </c>
       <c r="BJ22" s="0">
-        <v>11</v>
+        <v>10.375</v>
       </c>
       <c r="BK22" s="0">
-        <v>825000</v>
+        <v>778125</v>
       </c>
       <c r="BL22" s="0">
-        <v>0.82499999999999996</v>
+        <v>0.77812499999999996</v>
       </c>
       <c r="BM22" s="0">
-        <v>2750</v>
+        <v>2593.75</v>
       </c>
       <c r="BN22" s="0">
-        <v>0.0027499999999999998</v>
+        <v>0.0025937499999999997</v>
       </c>
       <c r="BR22" s="0">
-        <v>76.099999999999994</v>
+        <v>75.5</v>
       </c>
       <c r="BS22" s="0">
-        <v>5707500</v>
+        <v>5662500</v>
       </c>
       <c r="BT22" s="0">
-        <v>5.7074999999999996</v>
+        <v>5.6624999999999996</v>
       </c>
       <c r="BU22" s="0">
-        <v>-3.0999999999999943</v>
+        <v>-2.875</v>
       </c>
       <c r="BV22" s="0">
-        <v>-232499.99999999956</v>
+        <v>-215625</v>
       </c>
       <c r="BW22" s="0">
-        <v>-0.23249999999999957</v>
+        <v>-0.21562499999999998</v>
       </c>
       <c r="BX22" s="0">
-        <v>-774.99999999999852</v>
+        <v>-718.75</v>
       </c>
       <c r="BY22" s="0">
-        <v>-0.00077499999999999856</v>
+        <v>-0.00071874999999999999</v>
       </c>
       <c r="CC22" s="0">
-        <v>140.90000000000001</v>
+        <v>135.875</v>
       </c>
       <c r="CD22" s="0">
-        <v>10567500</v>
+        <v>10190625</v>
       </c>
       <c r="CE22" s="0">
-        <v>10.567500000000001</v>
+        <v>10.190624999999999</v>
       </c>
       <c r="CF22" s="0">
-        <v>4.7249999999999943</v>
+        <v>9</v>
       </c>
       <c r="CG22" s="0">
-        <v>354374.99999999959</v>
+        <v>675000</v>
       </c>
       <c r="CH22" s="0">
-        <v>0.35437499999999955</v>
+        <v>0.67499999999999993</v>
       </c>
       <c r="CI22" s="0">
-        <v>1181.2499999999986</v>
+        <v>2250</v>
       </c>
       <c r="CJ22" s="0">
-        <v>0.0011812499999999985</v>
+        <v>0.0022499999999999998</v>
       </c>
       <c r="CN22" s="0">
-        <v>159.30000000000001</v>
+        <v>158.80000000000001</v>
       </c>
       <c r="CO22" s="0">
-        <v>11947500</v>
+        <v>11910000</v>
       </c>
       <c r="CP22" s="0">
-        <v>11.9475</v>
+        <v>11.91</v>
       </c>
       <c r="CQ22" s="0">
-        <v>-0.050000000000011369</v>
+        <v>-0.63333333333332575</v>
       </c>
       <c r="CR22" s="0">
-        <v>-3750.0000000008527</v>
+        <v>-47499.999999999432</v>
       </c>
       <c r="CS22" s="0">
-        <v>-0.0037500000000008525</v>
+        <v>-0.047499999999999432</v>
       </c>
       <c r="CT22" s="0">
-        <v>-12.500000000002842</v>
+        <v>-158.33333333333144</v>
       </c>
       <c r="CU22" s="0">
-        <v>-1.2500000000002842e-05</v>
+        <v>-0.00015833333333333143</v>
       </c>
       <c r="CY22" s="0">
-        <v>144.875</v>
+        <v>144.125</v>
       </c>
       <c r="CZ22" s="0">
-        <v>10865625</v>
+        <v>10809375</v>
       </c>
       <c r="DA22" s="0">
-        <v>10.865625</v>
+        <v>10.809374999999999</v>
       </c>
       <c r="DB22" s="0">
-        <v>10.75</v>
+        <v>11.708333333333314</v>
       </c>
       <c r="DC22" s="0">
-        <v>806250</v>
+        <v>878124.9999999986</v>
       </c>
       <c r="DD22" s="0">
-        <v>0.80625000000000002</v>
+        <v>0.8781249999999986</v>
       </c>
       <c r="DE22" s="0">
-        <v>2687.5</v>
+        <v>2927.0833333333285</v>
       </c>
       <c r="DF22" s="0">
-        <v>0.0026875000000000002</v>
+        <v>0.0029270833333333288</v>
       </c>
     </row>
     <row r="23">
@@ -10572,205 +10572,205 @@
         <v>717</v>
       </c>
       <c r="D27" s="0">
-        <v>151.5</v>
+        <v>149.375</v>
       </c>
       <c r="E27" s="0">
-        <v>11362500</v>
+        <v>11203125</v>
       </c>
       <c r="F27" s="0">
-        <v>11.362499999999999</v>
+        <v>11.203125</v>
       </c>
       <c r="G27" s="0">
-        <v>2.875</v>
+        <v>4.625</v>
       </c>
       <c r="H27" s="0">
-        <v>215625</v>
+        <v>346875</v>
       </c>
       <c r="I27" s="0">
-        <v>0.21562499999999998</v>
+        <v>0.34687499999999999</v>
       </c>
       <c r="J27" s="0">
-        <v>718.75</v>
+        <v>1156.25</v>
       </c>
       <c r="K27" s="0">
-        <v>0.00071874999999999999</v>
+        <v>0.0011562499999999999</v>
       </c>
       <c r="O27" s="0">
-        <v>142.875</v>
+        <v>141.375</v>
       </c>
       <c r="P27" s="0">
-        <v>10715625</v>
+        <v>10603125</v>
       </c>
       <c r="Q27" s="0">
-        <v>10.715624999999999</v>
+        <v>10.603125</v>
       </c>
       <c r="R27" s="0">
-        <v>9.25</v>
+        <v>7.625</v>
       </c>
       <c r="S27" s="0">
-        <v>693750</v>
+        <v>571875</v>
       </c>
       <c r="T27" s="0">
-        <v>0.69374999999999998</v>
+        <v>0.57187500000000002</v>
       </c>
       <c r="U27" s="0">
-        <v>2312.5</v>
+        <v>1906.25</v>
       </c>
       <c r="V27" s="0">
-        <v>0.0023124999999999999</v>
+        <v>0.0019062500000000002</v>
       </c>
       <c r="Z27" s="0">
-        <v>82.333333333333343</v>
+        <v>77.125</v>
       </c>
       <c r="AA27" s="0">
-        <v>6175000.0000000009</v>
+        <v>5784375</v>
       </c>
       <c r="AB27" s="0">
-        <v>6.1750000000000007</v>
+        <v>5.7843749999999998</v>
       </c>
       <c r="AC27" s="0">
-        <v>-9.9583333333333428</v>
+        <v>-7.125</v>
       </c>
       <c r="AD27" s="0">
-        <v>-746875.0000000007</v>
+        <v>-534375</v>
       </c>
       <c r="AE27" s="0">
-        <v>-0.74687500000000073</v>
+        <v>-0.53437499999999993</v>
       </c>
       <c r="AF27" s="0">
-        <v>-2489.5833333333358</v>
+        <v>-1781.25</v>
       </c>
       <c r="AG27" s="0">
-        <v>-0.0024895833333333358</v>
+        <v>-0.0017812499999999998</v>
       </c>
       <c r="AK27" s="0">
-        <v>150.75</v>
+        <v>152</v>
       </c>
       <c r="AL27" s="0">
-        <v>11306250</v>
+        <v>11400000</v>
       </c>
       <c r="AM27" s="0">
-        <v>11.30625</v>
+        <v>11.4</v>
       </c>
       <c r="AN27" s="0">
+        <v>3.0833333333333144</v>
+      </c>
+      <c r="AO27" s="0">
+        <v>231249.99999999857</v>
+      </c>
+      <c r="AP27" s="0">
+        <v>0.23124999999999857</v>
+      </c>
+      <c r="AQ27" s="0">
+        <v>770.8333333333286</v>
+      </c>
+      <c r="AR27" s="0">
+        <v>0.00077083333333332856</v>
+      </c>
+      <c r="AV27" s="0">
+        <v>152</v>
+      </c>
+      <c r="AW27" s="0">
+        <v>11400000</v>
+      </c>
+      <c r="AX27" s="0">
+        <v>11.4</v>
+      </c>
+      <c r="AY27" s="0">
         <v>5.4166666666666856</v>
       </c>
-      <c r="AO27" s="0">
+      <c r="AZ27" s="0">
         <v>406250.0000000014</v>
       </c>
-      <c r="AP27" s="0">
+      <c r="BA27" s="0">
         <v>0.40625000000000139</v>
       </c>
-      <c r="AQ27" s="0">
+      <c r="BB27" s="0">
         <v>1354.1666666666713</v>
       </c>
-      <c r="AR27" s="0">
+      <c r="BC27" s="0">
         <v>0.0013541666666666713</v>
       </c>
-      <c r="AV27" s="0">
-        <v>153.16666666666669</v>
-      </c>
-      <c r="AW27" s="0">
-        <v>11487500.000000002</v>
-      </c>
-      <c r="AX27" s="0">
-        <v>11.487500000000001</v>
-      </c>
-      <c r="AY27" s="0">
-        <v>5</v>
-      </c>
-      <c r="AZ27" s="0">
-        <v>375000</v>
-      </c>
-      <c r="BA27" s="0">
-        <v>0.375</v>
-      </c>
-      <c r="BB27" s="0">
-        <v>1250</v>
-      </c>
-      <c r="BC27" s="0">
-        <v>0.00125</v>
-      </c>
       <c r="BG27" s="0">
-        <v>142.30000000000001</v>
+        <v>140.41666666666666</v>
       </c>
       <c r="BH27" s="0">
-        <v>10672500</v>
+        <v>10531250</v>
       </c>
       <c r="BI27" s="0">
-        <v>10.672500000000001</v>
+        <v>10.531249999999998</v>
       </c>
       <c r="BJ27" s="0">
-        <v>4.5749999999999886</v>
+        <v>5.8333333333333428</v>
       </c>
       <c r="BK27" s="0">
-        <v>343124.99999999913</v>
+        <v>437500.0000000007</v>
       </c>
       <c r="BL27" s="0">
-        <v>0.34312499999999913</v>
+        <v>0.43750000000000072</v>
       </c>
       <c r="BM27" s="0">
-        <v>1143.749999999997</v>
+        <v>1458.3333333333358</v>
       </c>
       <c r="BN27" s="0">
-        <v>0.001143749999999997</v>
+        <v>0.0014583333333333358</v>
       </c>
       <c r="BR27" s="0">
-        <v>78.833333333333343</v>
+        <v>73.25</v>
       </c>
       <c r="BS27" s="0">
-        <v>5912500.0000000009</v>
+        <v>5493750</v>
       </c>
       <c r="BT27" s="0">
-        <v>5.9125000000000005</v>
+        <v>5.4937499999999995</v>
       </c>
       <c r="BU27" s="0">
-        <v>-2.7333333333333485</v>
+        <v>2.25</v>
       </c>
       <c r="BV27" s="0">
-        <v>-205000.00000000114</v>
+        <v>168750</v>
       </c>
       <c r="BW27" s="0">
-        <v>-0.20500000000000113</v>
+        <v>0.16874999999999998</v>
       </c>
       <c r="BX27" s="0">
-        <v>-683.33333333333712</v>
+        <v>562.5</v>
       </c>
       <c r="BY27" s="0">
-        <v>-0.00068333333333333711</v>
+        <v>0.00056249999999999996</v>
       </c>
       <c r="CC27" s="0">
-        <v>132.125</v>
+        <v>131.5</v>
       </c>
       <c r="CD27" s="0">
-        <v>9909375</v>
+        <v>9862500</v>
       </c>
       <c r="CE27" s="0">
-        <v>9.9093749999999989</v>
+        <v>9.8624999999999989</v>
       </c>
       <c r="CF27" s="0">
-        <v>8.7750000000000057</v>
+        <v>4.375</v>
       </c>
       <c r="CG27" s="0">
-        <v>658125.00000000047</v>
+        <v>328125</v>
       </c>
       <c r="CH27" s="0">
-        <v>0.6581250000000004</v>
+        <v>0.328125</v>
       </c>
       <c r="CI27" s="0">
-        <v>2193.7500000000014</v>
+        <v>1093.75</v>
       </c>
       <c r="CJ27" s="0">
-        <v>0.0021937500000000013</v>
+        <v>0.0010937500000000001</v>
       </c>
       <c r="CN27" s="0">
-        <v>149.80000000000001</v>
+        <v>149.30000000000001</v>
       </c>
       <c r="CO27" s="0">
-        <v>11235000</v>
+        <v>11197500</v>
       </c>
       <c r="CP27" s="0">
-        <v>11.235000000000001</v>
+        <v>11.1975</v>
       </c>
       <c r="CQ27" s="0">
         <v>9.5</v>
@@ -10788,28 +10788,28 @@
         <v>0.0023749999999999999</v>
       </c>
       <c r="CY27" s="0">
-        <v>138.16666666666666</v>
+        <v>138.83333333333334</v>
       </c>
       <c r="CZ27" s="0">
-        <v>10362500</v>
+        <v>10412500</v>
       </c>
       <c r="DA27" s="0">
-        <v>10.362499999999999</v>
+        <v>10.4125</v>
       </c>
       <c r="DB27" s="0">
-        <v>6.7083333333333428</v>
+        <v>5.2916666666666572</v>
       </c>
       <c r="DC27" s="0">
-        <v>503125.0000000007</v>
+        <v>396874.9999999993</v>
       </c>
       <c r="DD27" s="0">
-        <v>0.50312500000000071</v>
+        <v>0.39687499999999926</v>
       </c>
       <c r="DE27" s="0">
-        <v>1677.0833333333358</v>
+        <v>1322.9166666666642</v>
       </c>
       <c r="DF27" s="0">
-        <v>0.0016770833333333358</v>
+        <v>0.0013229166666666641</v>
       </c>
     </row>
     <row r="28">
@@ -11552,181 +11552,181 @@
         <v>837</v>
       </c>
       <c r="D32" s="0">
-        <v>141.625</v>
+        <v>140.30000000000001</v>
       </c>
       <c r="E32" s="0">
-        <v>10621875</v>
+        <v>10522500</v>
       </c>
       <c r="F32" s="0">
-        <v>10.621874999999999</v>
+        <v>10.522500000000001</v>
       </c>
       <c r="G32" s="0">
-        <v>9.875</v>
+        <v>9.0749999999999886</v>
       </c>
       <c r="H32" s="0">
-        <v>740625</v>
+        <v>680624.99999999919</v>
       </c>
       <c r="I32" s="0">
-        <v>0.74062499999999998</v>
+        <v>0.68062499999999915</v>
       </c>
       <c r="J32" s="0">
-        <v>2468.75</v>
+        <v>2268.7499999999973</v>
       </c>
       <c r="K32" s="0">
-        <v>0.00246875</v>
+        <v>0.0022687499999999973</v>
       </c>
       <c r="O32" s="0">
-        <v>135.5</v>
+        <v>134.375</v>
       </c>
       <c r="P32" s="0">
-        <v>10162500</v>
+        <v>10078125</v>
       </c>
       <c r="Q32" s="0">
-        <v>10.1625</v>
+        <v>10.078125</v>
       </c>
       <c r="R32" s="0">
-        <v>7.375</v>
+        <v>7</v>
       </c>
       <c r="S32" s="0">
-        <v>553125</v>
+        <v>525000</v>
       </c>
       <c r="T32" s="0">
-        <v>0.55312499999999998</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="U32" s="0">
-        <v>1843.75</v>
+        <v>1750</v>
       </c>
       <c r="V32" s="0">
-        <v>0.0018437499999999999</v>
+        <v>0.00175</v>
       </c>
       <c r="Z32" s="0">
-        <v>73.625</v>
+        <v>74.5</v>
       </c>
       <c r="AA32" s="0">
-        <v>5521875</v>
+        <v>5587500</v>
       </c>
       <c r="AB32" s="0">
-        <v>5.5218749999999996</v>
+        <v>5.5874999999999995</v>
       </c>
       <c r="AC32" s="0">
-        <v>8.7083333333333428</v>
+        <v>2.625</v>
       </c>
       <c r="AD32" s="0">
-        <v>653125.0000000007</v>
+        <v>196875</v>
       </c>
       <c r="AE32" s="0">
-        <v>0.65312500000000073</v>
+        <v>0.19687499999999999</v>
       </c>
       <c r="AF32" s="0">
-        <v>2177.0833333333358</v>
+        <v>656.25</v>
       </c>
       <c r="AG32" s="0">
-        <v>0.002177083333333336</v>
+        <v>0.00065624999999999993</v>
       </c>
       <c r="AK32" s="0">
-        <v>145</v>
+        <v>143.58333333333334</v>
       </c>
       <c r="AL32" s="0">
-        <v>10875000</v>
+        <v>10768750</v>
       </c>
       <c r="AM32" s="0">
-        <v>10.875</v>
+        <v>10.768750000000001</v>
       </c>
       <c r="AN32" s="0">
-        <v>5.75</v>
+        <v>8.4166666666666572</v>
       </c>
       <c r="AO32" s="0">
-        <v>431250</v>
+        <v>631249.9999999993</v>
       </c>
       <c r="AP32" s="0">
-        <v>0.43124999999999997</v>
+        <v>0.63124999999999931</v>
       </c>
       <c r="AQ32" s="0">
-        <v>1437.5</v>
+        <v>2104.1666666666642</v>
       </c>
       <c r="AR32" s="0">
-        <v>0.0014375</v>
+        <v>0.0021041666666666643</v>
       </c>
       <c r="AV32" s="0">
-        <v>146.16666666666666</v>
+        <v>146.58333333333334</v>
       </c>
       <c r="AW32" s="0">
-        <v>10962500</v>
+        <v>10993750</v>
       </c>
       <c r="AX32" s="0">
-        <v>10.962499999999999</v>
+        <v>10.99375</v>
       </c>
       <c r="AY32" s="0">
-        <v>7.0000000000000284</v>
+        <v>5.4166666666666572</v>
       </c>
       <c r="AZ32" s="0">
-        <v>525000.0000000021</v>
+        <v>406249.9999999993</v>
       </c>
       <c r="BA32" s="0">
-        <v>0.52500000000000213</v>
+        <v>0.40624999999999928</v>
       </c>
       <c r="BB32" s="0">
-        <v>1750.000000000007</v>
+        <v>1354.1666666666642</v>
       </c>
       <c r="BC32" s="0">
-        <v>0.0017500000000000072</v>
+        <v>0.0013541666666666643</v>
       </c>
       <c r="BG32" s="0">
-        <v>135</v>
+        <v>133.875</v>
       </c>
       <c r="BH32" s="0">
-        <v>10125000</v>
+        <v>10040625</v>
       </c>
       <c r="BI32" s="0">
-        <v>10.125</v>
+        <v>10.040625</v>
       </c>
       <c r="BJ32" s="0">
-        <v>7.3000000000000114</v>
+        <v>6.5416666666666572</v>
       </c>
       <c r="BK32" s="0">
-        <v>547500.00000000081</v>
+        <v>490624.9999999993</v>
       </c>
       <c r="BL32" s="0">
-        <v>0.54750000000000087</v>
+        <v>0.49062499999999926</v>
       </c>
       <c r="BM32" s="0">
-        <v>1825.0000000000027</v>
+        <v>1635.4166666666642</v>
       </c>
       <c r="BN32" s="0">
-        <v>0.0018250000000000028</v>
+        <v>0.0016354166666666641</v>
       </c>
       <c r="BR32" s="0">
-        <v>75.5</v>
+        <v>76.625</v>
       </c>
       <c r="BS32" s="0">
-        <v>5662500</v>
+        <v>5746875</v>
       </c>
       <c r="BT32" s="0">
-        <v>5.6624999999999996</v>
+        <v>5.7468750000000002</v>
       </c>
       <c r="BU32" s="0">
-        <v>3.3333333333333428</v>
+        <v>-3.375</v>
       </c>
       <c r="BV32" s="0">
-        <v>250000.0000000007</v>
+        <v>-253125</v>
       </c>
       <c r="BW32" s="0">
-        <v>0.25000000000000072</v>
+        <v>-0.25312499999999999</v>
       </c>
       <c r="BX32" s="0">
-        <v>833.33333333333564</v>
+        <v>-843.75</v>
       </c>
       <c r="BY32" s="0">
-        <v>0.00083333333333333577</v>
+        <v>-0.00084374999999999999</v>
       </c>
       <c r="CC32" s="0">
-        <v>127</v>
+        <v>126.375</v>
       </c>
       <c r="CD32" s="0">
-        <v>9525000</v>
+        <v>9478125</v>
       </c>
       <c r="CE32" s="0">
-        <v>9.5250000000000004</v>
+        <v>9.4781250000000004</v>
       </c>
       <c r="CF32" s="0">
         <v>5.125</v>
@@ -11744,52 +11744,52 @@
         <v>0.0012812499999999998</v>
       </c>
       <c r="CN32" s="0">
-        <v>144.375</v>
+        <v>143.5</v>
       </c>
       <c r="CO32" s="0">
-        <v>10828125</v>
+        <v>10762500</v>
       </c>
       <c r="CP32" s="0">
-        <v>10.828125</v>
+        <v>10.762499999999999</v>
       </c>
       <c r="CQ32" s="0">
-        <v>5.4250000000000114</v>
+        <v>5.8000000000000114</v>
       </c>
       <c r="CR32" s="0">
-        <v>406875.00000000087</v>
+        <v>435000.00000000087</v>
       </c>
       <c r="CS32" s="0">
-        <v>0.40687500000000082</v>
+        <v>0.43500000000000083</v>
       </c>
       <c r="CT32" s="0">
-        <v>1356.250000000003</v>
+        <v>1450.000000000003</v>
       </c>
       <c r="CU32" s="0">
-        <v>0.0013562500000000026</v>
+        <v>0.0014500000000000027</v>
       </c>
       <c r="CY32" s="0">
-        <v>133.875</v>
+        <v>135.16666666666666</v>
       </c>
       <c r="CZ32" s="0">
-        <v>10040625</v>
+        <v>10137500</v>
       </c>
       <c r="DA32" s="0">
-        <v>10.040625</v>
+        <v>10.137499999999999</v>
       </c>
       <c r="DB32" s="0">
-        <v>4.2916666666666572</v>
+        <v>3.6666666666666856</v>
       </c>
       <c r="DC32" s="0">
-        <v>321874.9999999993</v>
+        <v>275000.0000000014</v>
       </c>
       <c r="DD32" s="0">
-        <v>0.3218749999999993</v>
+        <v>0.27500000000000141</v>
       </c>
       <c r="DE32" s="0">
-        <v>1072.9166666666642</v>
+        <v>916.66666666667129</v>
       </c>
       <c r="DF32" s="0">
-        <v>0.0010729166666666643</v>
+        <v>0.00091666666666667142</v>
       </c>
     </row>
     <row r="33">
@@ -12532,244 +12532,244 @@
         <v>957</v>
       </c>
       <c r="D37" s="0">
-        <v>133.83333333333334</v>
+        <v>133.75</v>
       </c>
       <c r="E37" s="0">
-        <v>10037500</v>
+        <v>10031250</v>
       </c>
       <c r="F37" s="0">
-        <v>10.0375</v>
+        <v>10.03125</v>
       </c>
       <c r="G37" s="0">
-        <v>7.7916666666666572</v>
+        <v>6.5500000000000114</v>
       </c>
       <c r="H37" s="0">
-        <v>584374.9999999993</v>
+        <v>491250.00000000087</v>
       </c>
       <c r="I37" s="0">
-        <v>0.58437499999999931</v>
+        <v>0.49125000000000085</v>
       </c>
       <c r="J37" s="0">
-        <v>1947.9166666666642</v>
+        <v>1637.500000000003</v>
       </c>
       <c r="K37" s="0">
-        <v>0.0019479166666666644</v>
+        <v>0.0016375000000000029</v>
       </c>
       <c r="O37" s="0">
-        <v>132.16666666666666</v>
+        <v>131.5</v>
       </c>
       <c r="P37" s="0">
-        <v>9912500</v>
+        <v>9862500</v>
       </c>
       <c r="Q37" s="0">
-        <v>9.9124999999999996</v>
+        <v>9.8624999999999989</v>
       </c>
       <c r="R37" s="0">
-        <v>3.3333333333333428</v>
+        <v>2.875</v>
       </c>
       <c r="S37" s="0">
-        <v>250000.0000000007</v>
+        <v>215625</v>
       </c>
       <c r="T37" s="0">
-        <v>0.25000000000000072</v>
+        <v>0.21562499999999998</v>
       </c>
       <c r="U37" s="0">
-        <v>833.33333333333564</v>
+        <v>718.75</v>
       </c>
       <c r="V37" s="0">
-        <v>0.00083333333333333577</v>
+        <v>0.00071874999999999999</v>
       </c>
       <c r="Z37" s="0">
-        <v>76</v>
+        <v>70.625</v>
       </c>
       <c r="AA37" s="0">
-        <v>5700000</v>
+        <v>5296875</v>
       </c>
       <c r="AB37" s="0">
-        <v>5.7000000000000002</v>
+        <v>5.296875</v>
       </c>
       <c r="AC37" s="0">
-        <v>-2.375</v>
+        <v>3.875</v>
       </c>
       <c r="AD37" s="0">
-        <v>-178125</v>
+        <v>290625</v>
       </c>
       <c r="AE37" s="0">
-        <v>-0.17812500000000001</v>
+        <v>0.29062499999999997</v>
       </c>
       <c r="AF37" s="0">
-        <v>-593.75</v>
+        <v>968.75</v>
       </c>
       <c r="AG37" s="0">
-        <v>-0.00059374999999999999</v>
+        <v>0.00096874999999999988</v>
       </c>
       <c r="AK37" s="0">
-        <v>138.66666666666666</v>
+        <v>138.375</v>
       </c>
       <c r="AL37" s="0">
-        <v>10400000</v>
+        <v>10378125</v>
       </c>
       <c r="AM37" s="0">
-        <v>10.399999999999999</v>
+        <v>10.378124999999999</v>
       </c>
       <c r="AN37" s="0">
-        <v>6.3333333333333428</v>
+        <v>5.2083333333333428</v>
       </c>
       <c r="AO37" s="0">
-        <v>475000.0000000007</v>
+        <v>390625.0000000007</v>
       </c>
       <c r="AP37" s="0">
-        <v>0.4750000000000007</v>
+        <v>0.39062500000000072</v>
       </c>
       <c r="AQ37" s="0">
-        <v>1583.3333333333358</v>
+        <v>1302.0833333333358</v>
       </c>
       <c r="AR37" s="0">
-        <v>0.0015833333333333357</v>
+        <v>0.0013020833333333356</v>
       </c>
       <c r="AV37" s="0">
-        <v>142.83333333333334</v>
+        <v>142</v>
       </c>
       <c r="AW37" s="0">
-        <v>10712500</v>
+        <v>10650000</v>
       </c>
       <c r="AX37" s="0">
-        <v>10.7125</v>
+        <v>10.65</v>
       </c>
       <c r="AY37" s="0">
-        <v>3.3333333333333144</v>
+        <v>4.5833333333333428</v>
       </c>
       <c r="AZ37" s="0">
-        <v>249999.99999999857</v>
+        <v>343750.0000000007</v>
       </c>
       <c r="BA37" s="0">
-        <v>0.24999999999999856</v>
+        <v>0.34375000000000072</v>
       </c>
       <c r="BB37" s="0">
-        <v>833.3333333333286</v>
+        <v>1145.8333333333358</v>
       </c>
       <c r="BC37" s="0">
-        <v>0.00083333333333332851</v>
+        <v>0.0011458333333333357</v>
       </c>
       <c r="BG37" s="0">
-        <v>131.875</v>
+        <v>133.75</v>
       </c>
       <c r="BH37" s="0">
-        <v>9890625</v>
+        <v>10031250</v>
       </c>
       <c r="BI37" s="0">
-        <v>9.890625</v>
+        <v>10.03125</v>
       </c>
       <c r="BJ37" s="0">
-        <v>3.125</v>
+        <v>0.125</v>
       </c>
       <c r="BK37" s="0">
-        <v>234375</v>
+        <v>9375</v>
       </c>
       <c r="BL37" s="0">
-        <v>0.234375</v>
+        <v>0.0093749999999999997</v>
       </c>
       <c r="BM37" s="0">
-        <v>781.25</v>
+        <v>31.25</v>
       </c>
       <c r="BN37" s="0">
-        <v>0.00078125000000000004</v>
+        <v>3.1250000000000001e-05</v>
       </c>
       <c r="BR37" s="0">
-        <v>69.166666666666657</v>
+        <v>68.666666666666657</v>
       </c>
       <c r="BS37" s="0">
-        <v>5187499.9999999991</v>
+        <v>5149999.9999999991</v>
       </c>
       <c r="BT37" s="0">
-        <v>5.1874999999999991</v>
+        <v>5.1499999999999995</v>
       </c>
       <c r="BU37" s="0">
-        <v>6.3333333333333428</v>
+        <v>7.9583333333333428</v>
       </c>
       <c r="BV37" s="0">
-        <v>475000.0000000007</v>
+        <v>596875.0000000007</v>
       </c>
       <c r="BW37" s="0">
-        <v>0.4750000000000007</v>
+        <v>0.59687500000000071</v>
       </c>
       <c r="BX37" s="0">
-        <v>1583.3333333333358</v>
+        <v>1989.5833333333358</v>
       </c>
       <c r="BY37" s="0">
-        <v>0.0015833333333333357</v>
+        <v>0.0019895833333333358</v>
       </c>
       <c r="CC37" s="0">
-        <v>130.375</v>
+        <v>126.125</v>
       </c>
       <c r="CD37" s="0">
-        <v>9778125</v>
+        <v>9459375</v>
       </c>
       <c r="CE37" s="0">
-        <v>9.7781249999999993</v>
+        <v>9.4593749999999996</v>
       </c>
       <c r="CF37" s="0">
-        <v>-3.375</v>
+        <v>0.25</v>
       </c>
       <c r="CG37" s="0">
-        <v>-253125</v>
+        <v>18750</v>
       </c>
       <c r="CH37" s="0">
-        <v>-0.25312499999999999</v>
+        <v>0.018749999999999999</v>
       </c>
       <c r="CI37" s="0">
-        <v>-843.75</v>
+        <v>62.5</v>
       </c>
       <c r="CJ37" s="0">
-        <v>-0.00084374999999999999</v>
+        <v>6.2500000000000001e-05</v>
       </c>
       <c r="CN37" s="0">
-        <v>137.33333333333334</v>
+        <v>139.625</v>
       </c>
       <c r="CO37" s="0">
-        <v>10300000</v>
+        <v>10471875</v>
       </c>
       <c r="CP37" s="0">
-        <v>10.300000000000001</v>
+        <v>10.471874999999999</v>
       </c>
       <c r="CQ37" s="0">
-        <v>7.0416666666666572</v>
+        <v>3.875</v>
       </c>
       <c r="CR37" s="0">
-        <v>528124.9999999993</v>
+        <v>290625</v>
       </c>
       <c r="CS37" s="0">
-        <v>0.52812499999999929</v>
+        <v>0.29062499999999997</v>
       </c>
       <c r="CT37" s="0">
-        <v>1760.4166666666642</v>
+        <v>968.75</v>
       </c>
       <c r="CU37" s="0">
-        <v>0.0017604166666666643</v>
+        <v>0.00096874999999999988</v>
       </c>
       <c r="CY37" s="0">
-        <v>130.80000000000001</v>
+        <v>129.80000000000001</v>
       </c>
       <c r="CZ37" s="0">
-        <v>9810000</v>
+        <v>9735000</v>
       </c>
       <c r="DA37" s="0">
-        <v>9.8100000000000005</v>
+        <v>9.7350000000000012</v>
       </c>
       <c r="DB37" s="0">
-        <v>3.0749999999999886</v>
+        <v>5.3666666666666458</v>
       </c>
       <c r="DC37" s="0">
-        <v>230624.99999999916</v>
+        <v>402499.99999999843</v>
       </c>
       <c r="DD37" s="0">
-        <v>0.23062499999999914</v>
+        <v>0.40249999999999841</v>
       </c>
       <c r="DE37" s="0">
-        <v>768.74999999999716</v>
+        <v>1341.6666666666615</v>
       </c>
       <c r="DF37" s="0">
-        <v>0.00076874999999999708</v>
+        <v>0.0013416666666666614</v>
       </c>
     </row>
     <row r="38">
@@ -13512,244 +13512,244 @@
         <v>1077</v>
       </c>
       <c r="D42" s="0">
-        <v>132.5</v>
+        <v>133.75</v>
       </c>
       <c r="E42" s="0">
-        <v>9937500</v>
+        <v>10031250</v>
       </c>
       <c r="F42" s="0">
-        <v>9.9375</v>
+        <v>10.03125</v>
       </c>
       <c r="G42" s="0">
-        <v>1.3333333333333428</v>
+        <v>0</v>
       </c>
       <c r="H42" s="0">
-        <v>100000.00000000071</v>
+        <v>0</v>
       </c>
       <c r="I42" s="0">
-        <v>0.10000000000000071</v>
+        <v>0</v>
       </c>
       <c r="J42" s="0">
-        <v>333.3333333333357</v>
+        <v>0</v>
       </c>
       <c r="K42" s="0">
-        <v>0.00033333333333333571</v>
+        <v>0</v>
       </c>
       <c r="O42" s="0">
-        <v>130</v>
+        <v>128.90000000000001</v>
       </c>
       <c r="P42" s="0">
-        <v>9750000</v>
+        <v>9667500</v>
       </c>
       <c r="Q42" s="0">
-        <v>9.75</v>
+        <v>9.6675000000000004</v>
       </c>
       <c r="R42" s="0">
-        <v>2.1666666666666572</v>
+        <v>2.5999999999999943</v>
       </c>
       <c r="S42" s="0">
-        <v>162499.9999999993</v>
+        <v>194999.99999999956</v>
       </c>
       <c r="T42" s="0">
-        <v>0.16249999999999928</v>
+        <v>0.19499999999999956</v>
       </c>
       <c r="U42" s="0">
-        <v>541.66666666666436</v>
+        <v>649.99999999999852</v>
       </c>
       <c r="V42" s="0">
-        <v>0.00054166666666666426</v>
+        <v>0.00064999999999999856</v>
       </c>
       <c r="Z42" s="0">
-        <v>67.625</v>
+        <v>59.150000000000006</v>
       </c>
       <c r="AA42" s="0">
-        <v>5071875</v>
+        <v>4436250</v>
       </c>
       <c r="AB42" s="0">
-        <v>5.0718749999999995</v>
+        <v>4.4362500000000002</v>
       </c>
       <c r="AC42" s="0">
-        <v>8.375</v>
+        <v>11.474999999999994</v>
       </c>
       <c r="AD42" s="0">
-        <v>628125</v>
+        <v>860624.99999999953</v>
       </c>
       <c r="AE42" s="0">
-        <v>0.62812499999999993</v>
+        <v>0.86062499999999953</v>
       </c>
       <c r="AF42" s="0">
-        <v>2093.75</v>
+        <v>2868.7499999999986</v>
       </c>
       <c r="AG42" s="0">
-        <v>0.0020937499999999997</v>
+        <v>0.0028687499999999985</v>
       </c>
       <c r="AK42" s="0">
-        <v>137.69999999999999</v>
+        <v>138.125</v>
       </c>
       <c r="AL42" s="0">
-        <v>10327500</v>
+        <v>10359375</v>
       </c>
       <c r="AM42" s="0">
-        <v>10.327499999999999</v>
+        <v>10.359375</v>
       </c>
       <c r="AN42" s="0">
-        <v>0.96666666666666856</v>
+        <v>0.25</v>
       </c>
       <c r="AO42" s="0">
-        <v>72500.000000000146</v>
+        <v>18750</v>
       </c>
       <c r="AP42" s="0">
-        <v>0.072500000000000134</v>
+        <v>0.018749999999999999</v>
       </c>
       <c r="AQ42" s="0">
-        <v>241.66666666666714</v>
+        <v>62.5</v>
       </c>
       <c r="AR42" s="0">
-        <v>0.0002416666666666671</v>
+        <v>6.2500000000000001e-05</v>
       </c>
       <c r="AV42" s="0">
-        <v>139.5</v>
+        <v>136.15000000000001</v>
       </c>
       <c r="AW42" s="0">
-        <v>10462500</v>
+        <v>10211250</v>
       </c>
       <c r="AX42" s="0">
-        <v>10.4625</v>
+        <v>10.21125</v>
       </c>
       <c r="AY42" s="0">
-        <v>3.3333333333333428</v>
+        <v>5.8499999999999943</v>
       </c>
       <c r="AZ42" s="0">
-        <v>250000.0000000007</v>
+        <v>438749.99999999959</v>
       </c>
       <c r="BA42" s="0">
-        <v>0.25000000000000072</v>
+        <v>0.43874999999999958</v>
       </c>
       <c r="BB42" s="0">
-        <v>833.33333333333564</v>
+        <v>1462.4999999999986</v>
       </c>
       <c r="BC42" s="0">
-        <v>0.00083333333333333577</v>
+        <v>0.0014624999999999985</v>
       </c>
       <c r="BG42" s="0">
-        <v>127.25</v>
+        <v>126.375</v>
       </c>
       <c r="BH42" s="0">
-        <v>9543750</v>
+        <v>9478125</v>
       </c>
       <c r="BI42" s="0">
-        <v>9.5437499999999993</v>
+        <v>9.4781250000000004</v>
       </c>
       <c r="BJ42" s="0">
-        <v>4.625</v>
+        <v>7.375</v>
       </c>
       <c r="BK42" s="0">
-        <v>346875</v>
+        <v>553125</v>
       </c>
       <c r="BL42" s="0">
-        <v>0.34687499999999999</v>
+        <v>0.55312499999999998</v>
       </c>
       <c r="BM42" s="0">
-        <v>1156.25</v>
+        <v>1843.75</v>
       </c>
       <c r="BN42" s="0">
-        <v>0.0011562499999999999</v>
+        <v>0.0018437499999999999</v>
       </c>
       <c r="BR42" s="0">
-        <v>274</v>
+        <v>62.875</v>
       </c>
       <c r="BS42" s="0">
-        <v>20550000</v>
+        <v>4715625</v>
       </c>
       <c r="BT42" s="0">
-        <v>20.550000000000001</v>
+        <v>4.7156250000000002</v>
       </c>
       <c r="BU42" s="0">
-        <v>-204.83333333333334</v>
+        <v>5.7916666666666572</v>
       </c>
       <c r="BV42" s="0">
-        <v>-15362500</v>
+        <v>434374.9999999993</v>
       </c>
       <c r="BW42" s="0">
-        <v>-15.362500000000001</v>
+        <v>0.43437499999999929</v>
       </c>
       <c r="BX42" s="0">
-        <v>-51208.333333333336</v>
+        <v>1447.9166666666642</v>
       </c>
       <c r="BY42" s="0">
-        <v>-0.051208333333333335</v>
+        <v>0.0014479166666666642</v>
       </c>
       <c r="CC42" s="0">
-        <v>116.75</v>
+        <v>115.5</v>
       </c>
       <c r="CD42" s="0">
-        <v>8756250</v>
+        <v>8662500</v>
       </c>
       <c r="CE42" s="0">
-        <v>8.7562499999999996</v>
+        <v>8.6624999999999996</v>
       </c>
       <c r="CF42" s="0">
-        <v>13.625</v>
+        <v>10.625</v>
       </c>
       <c r="CG42" s="0">
-        <v>1021875</v>
+        <v>796875</v>
       </c>
       <c r="CH42" s="0">
-        <v>1.0218749999999999</v>
+        <v>0.796875</v>
       </c>
       <c r="CI42" s="0">
-        <v>3406.25</v>
+        <v>2656.25</v>
       </c>
       <c r="CJ42" s="0">
-        <v>0.0034062499999999996</v>
+        <v>0.0026562500000000002</v>
       </c>
       <c r="CN42" s="0">
-        <v>133</v>
+        <v>132.625</v>
       </c>
       <c r="CO42" s="0">
-        <v>9975000</v>
+        <v>9946875</v>
       </c>
       <c r="CP42" s="0">
-        <v>9.9749999999999996</v>
+        <v>9.9468750000000004</v>
       </c>
       <c r="CQ42" s="0">
-        <v>4.3333333333333428</v>
+        <v>7</v>
       </c>
       <c r="CR42" s="0">
-        <v>325000.0000000007</v>
+        <v>525000</v>
       </c>
       <c r="CS42" s="0">
-        <v>0.32500000000000068</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="CT42" s="0">
-        <v>1083.3333333333358</v>
+        <v>1750</v>
       </c>
       <c r="CU42" s="0">
-        <v>0.0010833333333333357</v>
+        <v>0.00175</v>
       </c>
       <c r="CY42" s="0">
-        <v>128.66666666666666</v>
+        <v>130.5</v>
       </c>
       <c r="CZ42" s="0">
-        <v>9650000</v>
+        <v>9787500</v>
       </c>
       <c r="DA42" s="0">
-        <v>9.6499999999999986</v>
+        <v>9.7874999999999996</v>
       </c>
       <c r="DB42" s="0">
-        <v>2.1333333333333542</v>
+        <v>-0.69999999999998863</v>
       </c>
       <c r="DC42" s="0">
-        <v>160000.00000000157</v>
+        <v>-52499.999999999149</v>
       </c>
       <c r="DD42" s="0">
-        <v>0.16000000000000156</v>
+        <v>-0.052499999999999145</v>
       </c>
       <c r="DE42" s="0">
-        <v>533.3333333333386</v>
+        <v>-174.99999999999716</v>
       </c>
       <c r="DF42" s="0">
-        <v>0.00053333333333333856</v>
+        <v>-0.00017499999999999715</v>
       </c>
     </row>
     <row r="43">
@@ -14492,244 +14492,244 @@
         <v>1197</v>
       </c>
       <c r="D47" s="0">
-        <v>126.125</v>
+        <v>125.69999999999999</v>
       </c>
       <c r="E47" s="0">
-        <v>9459375</v>
+        <v>9427500</v>
       </c>
       <c r="F47" s="0">
-        <v>9.4593749999999996</v>
+        <v>9.4274999999999984</v>
       </c>
       <c r="G47" s="0">
-        <v>6.375</v>
+        <v>8.0500000000000114</v>
       </c>
       <c r="H47" s="0">
-        <v>478125</v>
+        <v>603750.00000000081</v>
       </c>
       <c r="I47" s="0">
-        <v>0.47812499999999997</v>
+        <v>0.60375000000000079</v>
       </c>
       <c r="J47" s="0">
-        <v>1593.75</v>
+        <v>2012.5000000000027</v>
       </c>
       <c r="K47" s="0">
-        <v>0.0015937499999999999</v>
+        <v>0.0020125000000000026</v>
       </c>
       <c r="O47" s="0">
-        <v>120.75</v>
+        <v>120.125</v>
       </c>
       <c r="P47" s="0">
-        <v>9056250</v>
+        <v>9009375</v>
       </c>
       <c r="Q47" s="0">
-        <v>9.0562500000000004</v>
+        <v>9.0093750000000004</v>
       </c>
       <c r="R47" s="0">
-        <v>9.25</v>
+        <v>8.7750000000000057</v>
       </c>
       <c r="S47" s="0">
-        <v>693750</v>
+        <v>658125.00000000047</v>
       </c>
       <c r="T47" s="0">
-        <v>0.69374999999999998</v>
+        <v>0.6581250000000004</v>
       </c>
       <c r="U47" s="0">
-        <v>2312.5</v>
+        <v>2193.7500000000014</v>
       </c>
       <c r="V47" s="0">
-        <v>0.0023124999999999999</v>
+        <v>0.0021937500000000013</v>
       </c>
       <c r="Z47" s="0">
-        <v>60</v>
+        <v>60.166666666666657</v>
       </c>
       <c r="AA47" s="0">
-        <v>4500000</v>
+        <v>4512499.9999999991</v>
       </c>
       <c r="AB47" s="0">
-        <v>4.5</v>
+        <v>4.5124999999999993</v>
       </c>
       <c r="AC47" s="0">
-        <v>7.625</v>
+        <v>-1.0166666666666515</v>
       </c>
       <c r="AD47" s="0">
-        <v>571875</v>
+        <v>-76249.999999998865</v>
       </c>
       <c r="AE47" s="0">
-        <v>0.57187500000000002</v>
+        <v>-0.07624999999999886</v>
       </c>
       <c r="AF47" s="0">
-        <v>1906.25</v>
+        <v>-254.16666666666288</v>
       </c>
       <c r="AG47" s="0">
-        <v>0.0019062500000000002</v>
+        <v>-0.00025416666666666285</v>
       </c>
       <c r="AK47" s="0">
-        <v>127.66666666666666</v>
+        <v>127</v>
       </c>
       <c r="AL47" s="0">
-        <v>9575000</v>
+        <v>9525000</v>
       </c>
       <c r="AM47" s="0">
-        <v>9.5749999999999993</v>
+        <v>9.5250000000000004</v>
       </c>
       <c r="AN47" s="0">
-        <v>10.033333333333331</v>
+        <v>11.125</v>
       </c>
       <c r="AO47" s="0">
-        <v>752499.99999999988</v>
+        <v>834375</v>
       </c>
       <c r="AP47" s="0">
-        <v>0.75249999999999984</v>
+        <v>0.83437499999999998</v>
       </c>
       <c r="AQ47" s="0">
-        <v>2508.333333333333</v>
+        <v>2781.25</v>
       </c>
       <c r="AR47" s="0">
-        <v>0.0025083333333333329</v>
+        <v>0.0027812499999999999</v>
       </c>
       <c r="AV47" s="0">
-        <v>136.83333333333334</v>
+        <v>133.625</v>
       </c>
       <c r="AW47" s="0">
-        <v>10262500</v>
+        <v>10021875</v>
       </c>
       <c r="AX47" s="0">
-        <v>10.262500000000001</v>
+        <v>10.021875</v>
       </c>
       <c r="AY47" s="0">
-        <v>2.6666666666666572</v>
+        <v>2.5250000000000057</v>
       </c>
       <c r="AZ47" s="0">
-        <v>199999.9999999993</v>
+        <v>189375.00000000044</v>
       </c>
       <c r="BA47" s="0">
-        <v>0.19999999999999929</v>
+        <v>0.18937500000000043</v>
       </c>
       <c r="BB47" s="0">
-        <v>666.66666666666436</v>
+        <v>631.25000000000148</v>
       </c>
       <c r="BC47" s="0">
-        <v>0.00066666666666666426</v>
+        <v>0.00063125000000000149</v>
       </c>
       <c r="BG47" s="0">
-        <v>119.83333333333334</v>
+        <v>121.08333333333334</v>
       </c>
       <c r="BH47" s="0">
-        <v>8987500</v>
+        <v>9081250</v>
       </c>
       <c r="BI47" s="0">
-        <v>8.9875000000000007</v>
+        <v>9.0812500000000007</v>
       </c>
       <c r="BJ47" s="0">
-        <v>7.4166666666666572</v>
+        <v>5.2916666666666572</v>
       </c>
       <c r="BK47" s="0">
-        <v>556249.9999999993</v>
+        <v>396874.9999999993</v>
       </c>
       <c r="BL47" s="0">
-        <v>0.55624999999999925</v>
+        <v>0.39687499999999926</v>
       </c>
       <c r="BM47" s="0">
-        <v>1854.1666666666642</v>
+        <v>1322.9166666666642</v>
       </c>
       <c r="BN47" s="0">
-        <v>0.0018541666666666641</v>
+        <v>0.0013229166666666641</v>
       </c>
       <c r="BR47" s="0">
-        <v>274</v>
+        <v>60.166666666666657</v>
       </c>
       <c r="BS47" s="0">
-        <v>20550000</v>
+        <v>4512499.9999999991</v>
       </c>
       <c r="BT47" s="0">
-        <v>20.550000000000001</v>
+        <v>4.5124999999999993</v>
       </c>
       <c r="BU47" s="0">
-        <v>0</v>
+        <v>2.7083333333333428</v>
       </c>
       <c r="BV47" s="0">
-        <v>0</v>
+        <v>203125.0000000007</v>
       </c>
       <c r="BW47" s="0">
-        <v>0</v>
+        <v>0.20312500000000069</v>
       </c>
       <c r="BX47" s="0">
-        <v>0</v>
+        <v>677.08333333333564</v>
       </c>
       <c r="BY47" s="0">
-        <v>0</v>
+        <v>0.00067708333333333563</v>
       </c>
       <c r="CC47" s="0">
-        <v>110.25</v>
+        <v>111.75</v>
       </c>
       <c r="CD47" s="0">
-        <v>8268750</v>
+        <v>8381250</v>
       </c>
       <c r="CE47" s="0">
-        <v>8.2687499999999989</v>
+        <v>8.3812499999999996</v>
       </c>
       <c r="CF47" s="0">
-        <v>6.5</v>
+        <v>3.75</v>
       </c>
       <c r="CG47" s="0">
-        <v>487500</v>
+        <v>281250</v>
       </c>
       <c r="CH47" s="0">
-        <v>0.48749999999999999</v>
+        <v>0.28125</v>
       </c>
       <c r="CI47" s="0">
-        <v>1625</v>
+        <v>937.5</v>
       </c>
       <c r="CJ47" s="0">
-        <v>0.0016249999999999999</v>
+        <v>0.00093749999999999997</v>
       </c>
       <c r="CN47" s="0">
-        <v>125.5</v>
+        <v>126.66666666666666</v>
       </c>
       <c r="CO47" s="0">
-        <v>9412500</v>
+        <v>9500000</v>
       </c>
       <c r="CP47" s="0">
-        <v>9.4124999999999996</v>
+        <v>9.4999999999999982</v>
       </c>
       <c r="CQ47" s="0">
-        <v>7.5</v>
+        <v>5.9583333333333428</v>
       </c>
       <c r="CR47" s="0">
-        <v>562500</v>
+        <v>446875.0000000007</v>
       </c>
       <c r="CS47" s="0">
-        <v>0.5625</v>
+        <v>0.44687500000000069</v>
       </c>
       <c r="CT47" s="0">
-        <v>1875</v>
+        <v>1489.5833333333358</v>
       </c>
       <c r="CU47" s="0">
-        <v>0.0018749999999999999</v>
+        <v>0.0014895833333333356</v>
       </c>
       <c r="CY47" s="0">
-        <v>116</v>
+        <v>116.125</v>
       </c>
       <c r="CZ47" s="0">
-        <v>8700000</v>
+        <v>8709375</v>
       </c>
       <c r="DA47" s="0">
-        <v>8.6999999999999993</v>
+        <v>8.7093749999999996</v>
       </c>
       <c r="DB47" s="0">
-        <v>12.666666666666657</v>
+        <v>14.375</v>
       </c>
       <c r="DC47" s="0">
-        <v>949999.9999999993</v>
+        <v>1078125</v>
       </c>
       <c r="DD47" s="0">
-        <v>0.94999999999999929</v>
+        <v>1.078125</v>
       </c>
       <c r="DE47" s="0">
-        <v>3166.6666666666642</v>
+        <v>3593.75</v>
       </c>
       <c r="DF47" s="0">
-        <v>0.0031666666666666644</v>
+        <v>0.0035937500000000002</v>
       </c>
     </row>
     <row r="48">
@@ -15472,244 +15472,244 @@
         <v>1317</v>
       </c>
       <c r="D52" s="0">
-        <v>276</v>
+        <v>117.625</v>
       </c>
       <c r="E52" s="0">
-        <v>20700000</v>
+        <v>8821875</v>
       </c>
       <c r="F52" s="0">
-        <v>20.699999999999999</v>
+        <v>8.8218750000000004</v>
       </c>
       <c r="G52" s="0">
-        <v>-149.875</v>
+        <v>8.0749999999999886</v>
       </c>
       <c r="H52" s="0">
-        <v>-11240625</v>
+        <v>605624.99999999919</v>
       </c>
       <c r="I52" s="0">
-        <v>-11.240625</v>
+        <v>0.60562499999999908</v>
       </c>
       <c r="J52" s="0">
-        <v>-37468.75</v>
+        <v>2018.7499999999973</v>
       </c>
       <c r="K52" s="0">
-        <v>-0.037468750000000002</v>
+        <v>0.0020187499999999971</v>
       </c>
       <c r="O52" s="0">
-        <v>114.25</v>
+        <v>114.83333333333334</v>
       </c>
       <c r="P52" s="0">
-        <v>8568750</v>
+        <v>8612500</v>
       </c>
       <c r="Q52" s="0">
-        <v>8.5687499999999996</v>
+        <v>8.6125000000000007</v>
       </c>
       <c r="R52" s="0">
-        <v>6.5</v>
+        <v>5.2916666666666572</v>
       </c>
       <c r="S52" s="0">
-        <v>487500</v>
+        <v>396874.9999999993</v>
       </c>
       <c r="T52" s="0">
-        <v>0.48749999999999999</v>
+        <v>0.39687499999999926</v>
       </c>
       <c r="U52" s="0">
-        <v>1625</v>
+        <v>1322.9166666666642</v>
       </c>
       <c r="V52" s="0">
-        <v>0.0016249999999999999</v>
+        <v>0.0013229166666666641</v>
       </c>
       <c r="Z52" s="0">
-        <v>277</v>
+        <v>52.550000000000011</v>
       </c>
       <c r="AA52" s="0">
-        <v>20775000</v>
+        <v>3941250.0000000009</v>
       </c>
       <c r="AB52" s="0">
-        <v>20.774999999999999</v>
+        <v>3.9412500000000006</v>
       </c>
       <c r="AC52" s="0">
-        <v>-217</v>
+        <v>7.6166666666666458</v>
       </c>
       <c r="AD52" s="0">
-        <v>-16275000</v>
+        <v>571249.99999999849</v>
       </c>
       <c r="AE52" s="0">
-        <v>-16.274999999999999</v>
+        <v>0.57124999999999837</v>
       </c>
       <c r="AF52" s="0">
-        <v>-54250</v>
+        <v>1904.1666666666615</v>
       </c>
       <c r="AG52" s="0">
-        <v>-0.054249999999999993</v>
+        <v>0.0019041666666666612</v>
       </c>
       <c r="AK52" s="0">
-        <v>277</v>
+        <v>123.75</v>
       </c>
       <c r="AL52" s="0">
-        <v>20775000</v>
+        <v>9281250</v>
       </c>
       <c r="AM52" s="0">
-        <v>20.774999999999999</v>
+        <v>9.28125</v>
       </c>
       <c r="AN52" s="0">
-        <v>-149.33333333333334</v>
+        <v>3.25</v>
       </c>
       <c r="AO52" s="0">
-        <v>-11200000</v>
+        <v>243750</v>
       </c>
       <c r="AP52" s="0">
-        <v>-11.200000000000001</v>
+        <v>0.24374999999999999</v>
       </c>
       <c r="AQ52" s="0">
-        <v>-37333.333333333336</v>
+        <v>812.5</v>
       </c>
       <c r="AR52" s="0">
-        <v>-0.037333333333333336</v>
+        <v>0.00081249999999999996</v>
       </c>
       <c r="AV52" s="0">
-        <v>126</v>
+        <v>127.875</v>
       </c>
       <c r="AW52" s="0">
-        <v>9450000</v>
+        <v>9590625</v>
       </c>
       <c r="AX52" s="0">
-        <v>9.4499999999999993</v>
+        <v>9.5906249999999993</v>
       </c>
       <c r="AY52" s="0">
-        <v>10.833333333333343</v>
+        <v>5.75</v>
       </c>
       <c r="AZ52" s="0">
-        <v>812500.0000000007</v>
+        <v>431250</v>
       </c>
       <c r="BA52" s="0">
-        <v>0.81250000000000067</v>
+        <v>0.43124999999999997</v>
       </c>
       <c r="BB52" s="0">
-        <v>2708.3333333333358</v>
+        <v>1437.5</v>
       </c>
       <c r="BC52" s="0">
-        <v>0.0027083333333333356</v>
+        <v>0.0014375</v>
       </c>
       <c r="BG52" s="0">
-        <v>113.875</v>
+        <v>112.58333333333334</v>
       </c>
       <c r="BH52" s="0">
-        <v>8540625</v>
+        <v>8443750</v>
       </c>
       <c r="BI52" s="0">
-        <v>8.5406250000000004</v>
+        <v>8.4437499999999996</v>
       </c>
       <c r="BJ52" s="0">
-        <v>5.9583333333333428</v>
+        <v>8.5</v>
       </c>
       <c r="BK52" s="0">
-        <v>446875.0000000007</v>
+        <v>637500</v>
       </c>
       <c r="BL52" s="0">
-        <v>0.44687500000000069</v>
+        <v>0.63749999999999996</v>
       </c>
       <c r="BM52" s="0">
-        <v>1489.5833333333358</v>
+        <v>2125</v>
       </c>
       <c r="BN52" s="0">
-        <v>0.0014895833333333356</v>
+        <v>0.0021249999999999997</v>
       </c>
       <c r="BR52" s="0">
-        <v>274</v>
+        <v>52.333333333333343</v>
       </c>
       <c r="BS52" s="0">
-        <v>20550000</v>
+        <v>3925000.0000000009</v>
       </c>
       <c r="BT52" s="0">
-        <v>20.550000000000001</v>
+        <v>3.9250000000000007</v>
       </c>
       <c r="BU52" s="0">
-        <v>0</v>
+        <v>7.8333333333333144</v>
       </c>
       <c r="BV52" s="0">
-        <v>0</v>
+        <v>587499.9999999986</v>
       </c>
       <c r="BW52" s="0">
-        <v>0</v>
+        <v>0.58749999999999858</v>
       </c>
       <c r="BX52" s="0">
-        <v>0</v>
+        <v>1958.3333333333287</v>
       </c>
       <c r="BY52" s="0">
-        <v>0</v>
+        <v>0.0019583333333333284</v>
       </c>
       <c r="CC52" s="0">
-        <v>109.75</v>
+        <v>106.15000000000001</v>
       </c>
       <c r="CD52" s="0">
-        <v>8231250</v>
+        <v>7961250</v>
       </c>
       <c r="CE52" s="0">
-        <v>8.2312499999999993</v>
+        <v>7.9612499999999997</v>
       </c>
       <c r="CF52" s="0">
-        <v>0.5</v>
+        <v>5.5999999999999943</v>
       </c>
       <c r="CG52" s="0">
-        <v>37500</v>
+        <v>419999.99999999959</v>
       </c>
       <c r="CH52" s="0">
-        <v>0.037499999999999999</v>
+        <v>0.41999999999999954</v>
       </c>
       <c r="CI52" s="0">
-        <v>125</v>
+        <v>1399.9999999999986</v>
       </c>
       <c r="CJ52" s="0">
-        <v>0.000125</v>
+        <v>0.0013999999999999985</v>
       </c>
       <c r="CN52" s="0">
-        <v>120</v>
+        <v>121.5</v>
       </c>
       <c r="CO52" s="0">
-        <v>9000000</v>
+        <v>9112500</v>
       </c>
       <c r="CP52" s="0">
-        <v>9</v>
+        <v>9.1124999999999989</v>
       </c>
       <c r="CQ52" s="0">
-        <v>5.5</v>
+        <v>5.1666666666666572</v>
       </c>
       <c r="CR52" s="0">
-        <v>412500</v>
+        <v>387499.9999999993</v>
       </c>
       <c r="CS52" s="0">
-        <v>0.41249999999999998</v>
+        <v>0.38749999999999929</v>
       </c>
       <c r="CT52" s="0">
-        <v>1375</v>
+        <v>1291.6666666666642</v>
       </c>
       <c r="CU52" s="0">
-        <v>0.0013749999999999999</v>
+        <v>0.0012916666666666643</v>
       </c>
       <c r="CY52" s="0">
-        <v>113.83333333333334</v>
+        <v>111.69999999999999</v>
       </c>
       <c r="CZ52" s="0">
-        <v>8537500</v>
+        <v>8377499.9999999991</v>
       </c>
       <c r="DA52" s="0">
-        <v>8.5374999999999996</v>
+        <v>8.3774999999999995</v>
       </c>
       <c r="DB52" s="0">
-        <v>2.1666666666666572</v>
+        <v>4.4250000000000114</v>
       </c>
       <c r="DC52" s="0">
-        <v>162499.9999999993</v>
+        <v>331875.00000000087</v>
       </c>
       <c r="DD52" s="0">
-        <v>0.16249999999999928</v>
+        <v>0.33187500000000086</v>
       </c>
       <c r="DE52" s="0">
-        <v>541.66666666666436</v>
+        <v>1106.250000000003</v>
       </c>
       <c r="DF52" s="0">
-        <v>0.00054166666666666426</v>
+        <v>0.0011062500000000028</v>
       </c>
     </row>
     <row r="53">
@@ -16452,244 +16452,244 @@
         <v>1437</v>
       </c>
       <c r="D57" s="0">
-        <v>276</v>
+        <v>112.75</v>
       </c>
       <c r="E57" s="0">
-        <v>20700000</v>
+        <v>8456250</v>
       </c>
       <c r="F57" s="0">
-        <v>20.699999999999999</v>
+        <v>8.4562499999999989</v>
       </c>
       <c r="G57" s="0">
-        <v>0</v>
+        <v>4.875</v>
       </c>
       <c r="H57" s="0">
-        <v>0</v>
+        <v>365625</v>
       </c>
       <c r="I57" s="0">
-        <v>0</v>
+        <v>0.36562499999999998</v>
       </c>
       <c r="J57" s="0">
-        <v>0</v>
+        <v>1218.75</v>
       </c>
       <c r="K57" s="0">
-        <v>0</v>
+        <v>0.00121875</v>
       </c>
       <c r="O57" s="0">
-        <v>111.5</v>
+        <v>110</v>
       </c>
       <c r="P57" s="0">
-        <v>8362500</v>
+        <v>8250000</v>
       </c>
       <c r="Q57" s="0">
-        <v>8.3624999999999989</v>
+        <v>8.25</v>
       </c>
       <c r="R57" s="0">
-        <v>2.75</v>
+        <v>4.8333333333333428</v>
       </c>
       <c r="S57" s="0">
-        <v>206250</v>
+        <v>362500.0000000007</v>
       </c>
       <c r="T57" s="0">
-        <v>0.20624999999999999</v>
+        <v>0.36250000000000071</v>
       </c>
       <c r="U57" s="0">
-        <v>687.5</v>
+        <v>1208.3333333333358</v>
       </c>
       <c r="V57" s="0">
-        <v>0.00068749999999999996</v>
+        <v>0.0012083333333333358</v>
       </c>
       <c r="Z57" s="0">
-        <v>277</v>
+        <v>56.75</v>
       </c>
       <c r="AA57" s="0">
-        <v>20775000</v>
+        <v>4256250</v>
       </c>
       <c r="AB57" s="0">
-        <v>20.774999999999999</v>
+        <v>4.2562499999999996</v>
       </c>
       <c r="AC57" s="0">
-        <v>0</v>
+        <v>-4.1999999999999886</v>
       </c>
       <c r="AD57" s="0">
-        <v>0</v>
+        <v>-314999.99999999913</v>
       </c>
       <c r="AE57" s="0">
-        <v>0</v>
+        <v>-0.31499999999999911</v>
       </c>
       <c r="AF57" s="0">
-        <v>0</v>
+        <v>-1049.999999999997</v>
       </c>
       <c r="AG57" s="0">
-        <v>0</v>
+        <v>-0.0010499999999999971</v>
       </c>
       <c r="AK57" s="0">
-        <v>277</v>
+        <v>118.5</v>
       </c>
       <c r="AL57" s="0">
-        <v>20775000</v>
+        <v>8887500</v>
       </c>
       <c r="AM57" s="0">
-        <v>20.774999999999999</v>
+        <v>8.8874999999999993</v>
       </c>
       <c r="AN57" s="0">
-        <v>0</v>
+        <v>5.25</v>
       </c>
       <c r="AO57" s="0">
-        <v>0</v>
+        <v>393750</v>
       </c>
       <c r="AP57" s="0">
-        <v>0</v>
+        <v>0.39374999999999999</v>
       </c>
       <c r="AQ57" s="0">
-        <v>0</v>
+        <v>1312.5</v>
       </c>
       <c r="AR57" s="0">
-        <v>0</v>
+        <v>0.0013124999999999999</v>
       </c>
       <c r="AV57" s="0">
-        <v>124</v>
+        <v>122.08333333333334</v>
       </c>
       <c r="AW57" s="0">
-        <v>9300000</v>
+        <v>9156250</v>
       </c>
       <c r="AX57" s="0">
-        <v>9.2999999999999989</v>
+        <v>9.15625</v>
       </c>
       <c r="AY57" s="0">
-        <v>2</v>
+        <v>5.7916666666666572</v>
       </c>
       <c r="AZ57" s="0">
-        <v>150000</v>
+        <v>434374.9999999993</v>
       </c>
       <c r="BA57" s="0">
-        <v>0.14999999999999999</v>
+        <v>0.43437499999999929</v>
       </c>
       <c r="BB57" s="0">
-        <v>500</v>
+        <v>1447.9166666666642</v>
       </c>
       <c r="BC57" s="0">
-        <v>0.00050000000000000001</v>
+        <v>0.0014479166666666642</v>
       </c>
       <c r="BG57" s="0">
-        <v>112</v>
+        <v>110.94999999999999</v>
       </c>
       <c r="BH57" s="0">
-        <v>8400000</v>
+        <v>8321249.9999999991</v>
       </c>
       <c r="BI57" s="0">
-        <v>8.4000000000000004</v>
+        <v>8.3212499999999991</v>
       </c>
       <c r="BJ57" s="0">
-        <v>1.875</v>
+        <v>1.6333333333333542</v>
       </c>
       <c r="BK57" s="0">
-        <v>140625</v>
+        <v>122500.00000000156</v>
       </c>
       <c r="BL57" s="0">
-        <v>0.140625</v>
+        <v>0.12250000000000155</v>
       </c>
       <c r="BM57" s="0">
-        <v>468.75</v>
+        <v>408.33333333333854</v>
       </c>
       <c r="BN57" s="0">
-        <v>0.00046874999999999998</v>
+        <v>0.00040833333333333851</v>
       </c>
       <c r="BR57" s="0">
-        <v>51</v>
+        <v>51.625</v>
       </c>
       <c r="BS57" s="0">
-        <v>3825000</v>
+        <v>3871875</v>
       </c>
       <c r="BT57" s="0">
-        <v>3.8249999999999997</v>
+        <v>3.8718749999999997</v>
       </c>
       <c r="BU57" s="0">
-        <v>223</v>
+        <v>0.70833333333334281</v>
       </c>
       <c r="BV57" s="0">
-        <v>16725000</v>
+        <v>53125.000000000713</v>
       </c>
       <c r="BW57" s="0">
-        <v>16.724999999999998</v>
+        <v>0.053125000000000706</v>
       </c>
       <c r="BX57" s="0">
-        <v>55750</v>
+        <v>177.0833333333357</v>
       </c>
       <c r="BY57" s="0">
-        <v>0.055749999999999994</v>
+        <v>0.00017708333333333568</v>
       </c>
       <c r="CC57" s="0">
-        <v>104.5</v>
+        <v>103.65000000000001</v>
       </c>
       <c r="CD57" s="0">
-        <v>7837500</v>
+        <v>7773750</v>
       </c>
       <c r="CE57" s="0">
-        <v>7.8374999999999995</v>
+        <v>7.7737499999999997</v>
       </c>
       <c r="CF57" s="0">
-        <v>5.25</v>
+        <v>2.5</v>
       </c>
       <c r="CG57" s="0">
-        <v>393750</v>
+        <v>187500</v>
       </c>
       <c r="CH57" s="0">
-        <v>0.39374999999999999</v>
+        <v>0.1875</v>
       </c>
       <c r="CI57" s="0">
-        <v>1312.5</v>
+        <v>625</v>
       </c>
       <c r="CJ57" s="0">
-        <v>0.0013124999999999999</v>
+        <v>0.00062500000000000001</v>
       </c>
       <c r="CN57" s="0">
-        <v>117</v>
+        <v>117.58333333333334</v>
       </c>
       <c r="CO57" s="0">
-        <v>8775000</v>
+        <v>8818750</v>
       </c>
       <c r="CP57" s="0">
-        <v>8.7750000000000004</v>
+        <v>8.8187499999999996</v>
       </c>
       <c r="CQ57" s="0">
-        <v>3</v>
+        <v>3.9166666666666572</v>
       </c>
       <c r="CR57" s="0">
-        <v>225000</v>
+        <v>293749.9999999993</v>
       </c>
       <c r="CS57" s="0">
-        <v>0.22499999999999998</v>
+        <v>0.29374999999999929</v>
       </c>
       <c r="CT57" s="0">
-        <v>750</v>
+        <v>979.16666666666436</v>
       </c>
       <c r="CU57" s="0">
-        <v>0.00074999999999999991</v>
+        <v>0.00097916666666666421</v>
       </c>
       <c r="CY57" s="0">
-        <v>105.33333333333334</v>
+        <v>105</v>
       </c>
       <c r="CZ57" s="0">
-        <v>7900000.0000000009</v>
+        <v>7875000</v>
       </c>
       <c r="DA57" s="0">
-        <v>7.9000000000000004</v>
+        <v>7.875</v>
       </c>
       <c r="DB57" s="0">
-        <v>8.5</v>
+        <v>6.6999999999999886</v>
       </c>
       <c r="DC57" s="0">
-        <v>637500</v>
+        <v>502499.99999999913</v>
       </c>
       <c r="DD57" s="0">
-        <v>0.63749999999999996</v>
+        <v>0.50249999999999917</v>
       </c>
       <c r="DE57" s="0">
-        <v>2125</v>
+        <v>1674.999999999997</v>
       </c>
       <c r="DF57" s="0">
-        <v>0.0021249999999999997</v>
+        <v>0.0016749999999999972</v>
       </c>
     </row>
     <row r="58">

</xml_diff>